<commit_message>
Optimize "remove" related function
</commit_message>
<xml_diff>
--- a/app/result.xlsx
+++ b/app/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QOC\MeshSimplification-Mobile\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41E6854-6BD3-476E-8E93-8D2DB8FA8A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFA83ED-124C-4FDC-BEEE-977F0CB98569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
   <si>
     <t>mesh0</t>
   </si>
@@ -904,6 +904,9 @@
   </si>
   <si>
     <t>Quadric Cost</t>
+  </si>
+  <si>
+    <t>Optimize "remove" parts</t>
   </si>
 </sst>
 </file>
@@ -1222,20 +1225,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C292"/>
+  <dimension ref="A1:D292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="D292" sqref="D292"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.28515625" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,8 +1248,11 @@
       <c r="C1">
         <v>27.341000000000001</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>26.645099999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1256,8 +1262,11 @@
       <c r="C2">
         <v>26.1479</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>25.4816</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1267,8 +1276,11 @@
       <c r="C3">
         <v>25.2638</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>24.590599999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1278,8 +1290,11 @@
       <c r="C4">
         <v>4.4989299999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>4.5028199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1289,8 +1304,11 @@
       <c r="C5">
         <v>2.91221</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2.8674400000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1300,8 +1318,11 @@
       <c r="C6">
         <v>2.3242400000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2.2815799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1311,8 +1332,11 @@
       <c r="C7">
         <v>1.6282300000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1.6057399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1322,8 +1346,11 @@
       <c r="C8">
         <v>3.5157699999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>3.4923999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1333,8 +1360,11 @@
       <c r="C9">
         <v>3.9782000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>3.9348299999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1344,8 +1374,11 @@
       <c r="C10">
         <v>2.06819</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2.0288900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1355,8 +1388,11 @@
       <c r="C11">
         <v>3.7271200000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>3.6890800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1366,8 +1402,11 @@
       <c r="C12">
         <v>1.6012500000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1.59019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1377,8 +1416,11 @@
       <c r="C13">
         <v>4.6410600000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>4.6019100000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1388,8 +1430,11 @@
       <c r="C14">
         <v>41.622199999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>40.738300000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1399,8 +1444,11 @@
       <c r="C15">
         <v>4.3907699999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>4.4015899999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1410,8 +1458,11 @@
       <c r="C16">
         <v>2.1508799999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>2.1289899999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1421,8 +1472,11 @@
       <c r="C17">
         <v>2.0928599999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>2.0671599999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1432,8 +1486,11 @@
       <c r="C18">
         <v>2.0119699999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>1.98336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1443,8 +1500,11 @@
       <c r="C19">
         <v>2.2934199999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>2.26986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1454,8 +1514,11 @@
       <c r="C20">
         <v>3.83094</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>3.79569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1465,8 +1528,11 @@
       <c r="C21">
         <v>3.0955499999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>3.0679400000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1476,8 +1542,11 @@
       <c r="C22">
         <v>1.49905</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1.4947299999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1487,8 +1556,11 @@
       <c r="C23">
         <v>2.7807599999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>2.7608700000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1498,8 +1570,11 @@
       <c r="C24">
         <v>3.4969999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>3.4636399999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1509,8 +1584,11 @@
       <c r="C25">
         <v>45.306399999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>44.277799999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1520,8 +1598,11 @@
       <c r="C26">
         <v>2.9416199999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>2.9484900000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1531,8 +1612,11 @@
       <c r="C27">
         <v>4.4091100000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>4.3599399999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1542,8 +1626,11 @@
       <c r="C28">
         <v>1.7259500000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>1.7057599999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1553,8 +1640,11 @@
       <c r="C29">
         <v>2.2028500000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>2.1858200000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1564,8 +1654,11 @@
       <c r="C30">
         <v>2.4250400000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>2.39106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1575,8 +1668,11 @@
       <c r="C31">
         <v>3.4330699999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>3.40544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1586,8 +1682,11 @@
       <c r="C32">
         <v>3.03328</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>3.0025499999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1597,8 +1696,11 @@
       <c r="C33">
         <v>2.2122700000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>2.18641</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1608,8 +1710,11 @@
       <c r="C34">
         <v>1.8293999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1.8025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1619,8 +1724,11 @@
       <c r="C35">
         <v>4.8842400000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>4.85677</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1630,8 +1738,11 @@
       <c r="C36">
         <v>24.6294</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>24.041899999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1641,8 +1752,11 @@
       <c r="C37">
         <v>4.03531</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>4.0254200000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1652,8 +1766,11 @@
       <c r="C38">
         <v>3.4533299999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>3.4244699999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1663,8 +1780,11 @@
       <c r="C39">
         <v>1.81301</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>1.7976399999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1674,8 +1794,11 @@
       <c r="C40">
         <v>3.4657499999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>3.41994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1685,8 +1808,11 @@
       <c r="C41">
         <v>2.3990399999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>2.3686199999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1696,8 +1822,11 @@
       <c r="C42">
         <v>2.6660400000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>2.6386400000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1707,8 +1836,11 @@
       <c r="C43">
         <v>2.5222600000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>2.47743</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1718,8 +1850,11 @@
       <c r="C44">
         <v>2.6183700000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>2.5812499999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1729,8 +1864,11 @@
       <c r="C45">
         <v>1.6916599999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>1.6752</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1740,8 +1878,11 @@
       <c r="C46">
         <v>2.6644000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>2.6452100000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1751,8 +1892,11 @@
       <c r="C47">
         <v>27.2684</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>26.5763</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1762,8 +1906,11 @@
       <c r="C48">
         <v>2.47838</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>2.4791699999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1773,8 +1920,11 @@
       <c r="C49">
         <v>2.9704899999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>2.9527999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1784,8 +1934,11 @@
       <c r="C50">
         <v>1.8615900000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>1.8435699999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1795,8 +1948,11 @@
       <c r="C51">
         <v>3.4366599999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>3.4011300000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1806,8 +1962,11 @@
       <c r="C52">
         <v>4.2097499999999997</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>4.1747399999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1817,8 +1976,11 @@
       <c r="C53">
         <v>3.1334399999999998</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>3.0841599999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1828,8 +1990,11 @@
       <c r="C54">
         <v>1.8411299999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>1.8150999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1839,8 +2004,11 @@
       <c r="C55">
         <v>2.8344</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>2.7978700000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1850,8 +2018,11 @@
       <c r="C56">
         <v>3.1980400000000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>3.1404100000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1861,8 +2032,11 @@
       <c r="C57">
         <v>2.5007899999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>2.4623900000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1872,8 +2046,11 @@
       <c r="C58">
         <v>24.5228</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>23.8401</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1883,8 +2060,11 @@
       <c r="C59">
         <v>3.7992699999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>3.7914400000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1894,8 +2074,11 @@
       <c r="C60">
         <v>1.86252</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>1.8464799999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1905,8 +2088,11 @@
       <c r="C61">
         <v>1.8154999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>1.81006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1916,8 +2102,11 @@
       <c r="C62">
         <v>3.60676</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>3.5753699999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1927,8 +2116,11 @@
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1938,8 +2130,11 @@
       <c r="C64">
         <v>3.3229099999999998</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>3.2844199999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1949,8 +2144,11 @@
       <c r="C65">
         <v>6.1877399999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>6.1429099999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1960,8 +2158,11 @@
       <c r="C66">
         <v>12.547599999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>12.4376</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1971,8 +2172,11 @@
       <c r="C67">
         <v>2.6048900000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>2.58833</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1982,8 +2186,11 @@
       <c r="C68">
         <v>2.3258100000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>2.31487</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1993,8 +2200,11 @@
       <c r="C69">
         <v>27.287199999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>26.574300000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2004,8 +2214,11 @@
       <c r="C70">
         <v>2.6869299999999998</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>2.6963499999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2015,8 +2228,11 @@
       <c r="C71">
         <v>1.65059</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>1.6382699999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2026,8 +2242,11 @@
       <c r="C72">
         <v>1.8659399999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>1.8500300000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2037,8 +2256,11 @@
       <c r="C73">
         <v>3.3409399999999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>3.3079999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2048,8 +2270,11 @@
       <c r="C74">
         <v>1.6601600000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>1.6420600000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2059,8 +2284,11 @@
       <c r="C75">
         <v>3.4276300000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>3.3986999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2070,8 +2298,11 @@
       <c r="C76">
         <v>3.0886800000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>3.0680999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2081,8 +2312,11 @@
       <c r="C77">
         <v>3.2032400000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>3.1776499999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2092,8 +2326,11 @@
       <c r="C78">
         <v>2.1478199999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>2.1153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2103,8 +2340,11 @@
       <c r="C79">
         <v>3.3278799999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>3.28227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2114,8 +2354,11 @@
       <c r="C80">
         <v>24.4602</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>23.785799999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2125,8 +2368,11 @@
       <c r="C81">
         <v>2.39303</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>2.4056500000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2136,8 +2382,11 @@
       <c r="C82">
         <v>2.1016300000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>2.0845600000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2147,8 +2396,11 @@
       <c r="C83">
         <v>2.9187500000000002</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>2.8949099999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2158,8 +2410,11 @@
       <c r="C84">
         <v>5.7110099999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>5.68546</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2169,8 +2424,11 @@
       <c r="C85">
         <v>3.6299000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>3.5775800000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2180,8 +2438,11 @@
       <c r="C86">
         <v>2.74987</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>2.7273999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2191,8 +2452,11 @@
       <c r="C87">
         <v>3.0342500000000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>3.0183300000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2202,8 +2466,11 @@
       <c r="C88">
         <v>2.9996700000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>2.9729899999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2213,8 +2480,11 @@
       <c r="C89">
         <v>1.71532</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>1.69614</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2224,8 +2494,11 @@
       <c r="C90">
         <v>3.0198100000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>3.0073500000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2235,8 +2508,11 @@
       <c r="C91">
         <v>27.1386</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>26.446200000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2246,8 +2522,11 @@
       <c r="C92">
         <v>2.5838100000000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>2.5889000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2257,8 +2536,11 @@
       <c r="C93">
         <v>1.91476</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>1.9086399999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2268,8 +2550,11 @@
       <c r="C94">
         <v>1.7865899999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>1.77345</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2279,8 +2564,11 @@
       <c r="C95">
         <v>3.6932999999999998</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>3.6530999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2290,8 +2578,11 @@
       <c r="C96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2301,8 +2592,11 @@
       <c r="C97">
         <v>3.1090499999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>3.0809600000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2312,8 +2606,11 @@
       <c r="C98">
         <v>3.2303000000000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>3.2081599999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2323,8 +2620,11 @@
       <c r="C99">
         <v>3.1639599999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>3.1449400000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2334,8 +2634,11 @@
       <c r="C100">
         <v>4.7826199999999996</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>4.7814100000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2345,8 +2648,11 @@
       <c r="C101">
         <v>1.9790399999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>1.9599</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2356,8 +2662,11 @@
       <c r="C102">
         <v>24.730599999999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>24.073399999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2367,8 +2676,11 @@
       <c r="C103">
         <v>5.1507500000000004</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>5.1394900000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2378,8 +2690,11 @@
       <c r="C104">
         <v>2.57701</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>2.5534300000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2389,8 +2704,11 @@
       <c r="C105">
         <v>2.47228</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>2.4323899999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2400,8 +2718,11 @@
       <c r="C106">
         <v>1.8265899999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>1.8106500000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2411,8 +2732,11 @@
       <c r="C107">
         <v>2.3859300000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>2.35406</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2422,8 +2746,11 @@
       <c r="C108">
         <v>3.0500600000000002</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>3.0243500000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2433,8 +2760,11 @@
       <c r="C109">
         <v>1.5558799999999999</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>1.5483100000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2444,8 +2774,11 @@
       <c r="C110">
         <v>1.9497899999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>1.9303399999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2455,8 +2788,11 @@
       <c r="C111">
         <v>3.1234999999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>3.1055100000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2466,8 +2802,11 @@
       <c r="C112">
         <v>2.98902</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>2.97994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2477,8 +2816,11 @@
       <c r="C113">
         <v>24.482199999999999</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>23.845199999999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2488,8 +2830,11 @@
       <c r="C114">
         <v>25.466100000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>24.825399999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2499,8 +2844,11 @@
       <c r="C115">
         <v>3.74254</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>3.7283499999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2510,8 +2858,11 @@
       <c r="C116">
         <v>2.7274799999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>2.7207499999999998</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2521,8 +2872,11 @@
       <c r="C117">
         <v>3.1853600000000002</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>3.1663899999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2532,8 +2886,11 @@
       <c r="C118">
         <v>2.4050699999999998</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>2.3652600000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2543,8 +2900,11 @@
       <c r="C119">
         <v>1.96166</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>1.93303</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2554,8 +2914,11 @@
       <c r="C120">
         <v>1.8119799999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>1.7952300000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2565,8 +2928,11 @@
       <c r="C121">
         <v>3.5432600000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>3.5342099999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2576,8 +2942,11 @@
       <c r="C122">
         <v>5.5486700000000004</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>5.4940199999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2587,8 +2956,11 @@
       <c r="C123">
         <v>10.2347</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>10.1309</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2598,8 +2970,11 @@
       <c r="C124">
         <v>3.3008799999999998</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>3.2804600000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2609,8 +2984,11 @@
       <c r="C125">
         <v>27.3444</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>26.666399999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2620,8 +2998,11 @@
       <c r="C126">
         <v>8.6627500000000008</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>8.5622900000000008</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2631,8 +3012,11 @@
       <c r="C127">
         <v>3.40367</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>3.3925299999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2642,8 +3026,11 @@
       <c r="C128">
         <v>3.6835</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>3.6659600000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2653,8 +3040,11 @@
       <c r="C129">
         <v>3.5421299999999998</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>3.5186700000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2664,8 +3054,11 @@
       <c r="C130">
         <v>1.9408300000000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>1.91648</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2675,8 +3068,11 @@
       <c r="C131">
         <v>13.351100000000001</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>13.2486</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2686,8 +3082,11 @@
       <c r="C132">
         <v>2.9127299999999998</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>2.8814000000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2697,8 +3096,11 @@
       <c r="C133">
         <v>4.4101100000000004</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>4.3886099999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2708,8 +3110,11 @@
       <c r="C134">
         <v>5.6444700000000001</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>5.5784500000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -2719,8 +3124,11 @@
       <c r="C135">
         <v>6.7019399999999996</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>6.6763300000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -2730,8 +3138,11 @@
       <c r="C136">
         <v>15.0465</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>14.668900000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -2741,8 +3152,11 @@
       <c r="C137">
         <v>11.532299999999999</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>11.4376</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -2752,8 +3166,11 @@
       <c r="C138">
         <v>6.2545500000000001</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>6.2072900000000004</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -2763,8 +3180,11 @@
       <c r="C139">
         <v>35.404499999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>35.215000000000003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -2774,8 +3194,11 @@
       <c r="C140">
         <v>33.280700000000003</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>33.198300000000003</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -2785,8 +3208,11 @@
       <c r="C141">
         <v>4.5665399999999998</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>4.5459500000000004</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -2796,8 +3222,11 @@
       <c r="C142">
         <v>6.6790599999999998</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>6.6336500000000003</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -2807,8 +3236,11 @@
       <c r="C143">
         <v>6.30884</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>6.25122</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -2818,8 +3250,11 @@
       <c r="C144">
         <v>2.2394099999999999</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <v>2.22126</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -2829,8 +3264,11 @@
       <c r="C145">
         <v>6.7274000000000003</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>6.6275000000000004</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -2840,8 +3278,11 @@
       <c r="C146">
         <v>2.8215300000000001</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>2.7867600000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -2851,8 +3292,11 @@
       <c r="C147">
         <v>27.223500000000001</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <v>26.515799999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -2862,8 +3306,11 @@
       <c r="C148">
         <v>9.3256399999999999</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148">
+        <v>9.28613</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -2873,8 +3320,11 @@
       <c r="C149">
         <v>7.8295000000000003</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149">
+        <v>7.7919499999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -2884,8 +3334,11 @@
       <c r="C150">
         <v>12.5533</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150">
+        <v>12.491899999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -2895,8 +3348,11 @@
       <c r="C151">
         <v>19.029499999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151">
+        <v>18.878</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -2906,8 +3362,11 @@
       <c r="C152">
         <v>2.77908</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>2.7795399999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -2917,8 +3376,11 @@
       <c r="C153">
         <v>5.75122</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153">
+        <v>5.6460800000000004</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -2928,8 +3390,11 @@
       <c r="C154">
         <v>5.2527299999999997</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154">
+        <v>5.2243500000000003</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -2939,8 +3404,11 @@
       <c r="C155">
         <v>6.4020400000000004</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155">
+        <v>6.3710500000000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -2950,8 +3418,11 @@
       <c r="C156">
         <v>8.5414600000000007</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>8.5020299999999995</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -2961,8 +3432,11 @@
       <c r="C157">
         <v>19.991399999999999</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157">
+        <v>19.9206</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -2972,8 +3446,11 @@
       <c r="C158">
         <v>27.712399999999999</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158">
+        <v>27.0181</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -2983,8 +3460,11 @@
       <c r="C159">
         <v>6.2848300000000004</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159">
+        <v>6.2792700000000004</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -2994,8 +3474,11 @@
       <c r="C160">
         <v>2.8815400000000002</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160">
+        <v>2.85866</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -3005,8 +3488,11 @@
       <c r="C161">
         <v>3.8851499999999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161">
+        <v>3.8473000000000002</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -3016,8 +3502,11 @@
       <c r="C162">
         <v>8.8733199999999997</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162">
+        <v>8.8353000000000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -3027,8 +3516,11 @@
       <c r="C163">
         <v>7.8735600000000003</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>7.7979099999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -3038,8 +3530,11 @@
       <c r="C164">
         <v>2.5117699999999998</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>2.5000399999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -3049,8 +3544,11 @@
       <c r="C165">
         <v>5.2784500000000003</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>5.2278799999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -3060,8 +3558,11 @@
       <c r="C166">
         <v>5.8090299999999999</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>5.7481900000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -3071,8 +3572,11 @@
       <c r="C167">
         <v>6.7922200000000004</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>6.7116899999999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -3082,8 +3586,11 @@
       <c r="C168">
         <v>5.7172599999999996</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>5.6660300000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -3093,8 +3600,11 @@
       <c r="C169">
         <v>42.147599999999997</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>40.985700000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -3104,8 +3614,11 @@
       <c r="C170">
         <v>8.5601299999999991</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>8.5641800000000003</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -3115,8 +3628,11 @@
       <c r="C171">
         <v>4.20967</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>4.1753299999999998</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -3126,8 +3642,11 @@
       <c r="C172">
         <v>2.3732099999999998</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172">
+        <v>2.3434200000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -3137,8 +3656,11 @@
       <c r="C173">
         <v>2.9239000000000002</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173">
+        <v>2.8887200000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -3148,8 +3670,11 @@
       <c r="C174">
         <v>4.4337099999999996</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174">
+        <v>4.3646099999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -3159,8 +3684,11 @@
       <c r="C175">
         <v>2.3983699999999999</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175">
+        <v>2.371</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -3170,8 +3698,11 @@
       <c r="C176">
         <v>5.1530500000000004</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>5.1053300000000004</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -3181,8 +3712,11 @@
       <c r="C177">
         <v>5.2321499999999999</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>5.1746100000000004</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -3192,8 +3726,11 @@
       <c r="C178">
         <v>4.2180299999999997</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>4.1764099999999997</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -3203,8 +3740,11 @@
       <c r="C179">
         <v>6.1894799999999996</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>6.1577500000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -3214,8 +3754,11 @@
       <c r="C180">
         <v>27.413699999999999</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180">
+        <v>26.677900000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -3225,8 +3768,11 @@
       <c r="C181">
         <v>4.0226899999999999</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181">
+        <v>4.0160200000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -3236,8 +3782,11 @@
       <c r="C182">
         <v>8.7779900000000008</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>8.7148900000000005</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -3247,8 +3796,11 @@
       <c r="C183">
         <v>3.0983800000000001</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183">
+        <v>3.0794299999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -3258,8 +3810,11 @@
       <c r="C184">
         <v>3.4877199999999999</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184">
+        <v>3.4619300000000002</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -3269,8 +3824,11 @@
       <c r="C185">
         <v>2.6038199999999998</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185">
+        <v>2.5861000000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -3280,8 +3838,11 @@
       <c r="C186">
         <v>5.2218299999999997</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186">
+        <v>5.1710900000000004</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -3291,8 +3852,11 @@
       <c r="C187">
         <v>2.1627999999999998</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187">
+        <v>2.12765</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -3302,8 +3866,11 @@
       <c r="C188">
         <v>6.1683399999999997</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188">
+        <v>6.1364999999999998</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -3313,8 +3880,11 @@
       <c r="C189">
         <v>1.66215</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189">
+        <v>1.6454500000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -3324,8 +3894,11 @@
       <c r="C190">
         <v>2.0270899999999998</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190">
+        <v>1.99495</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -3335,8 +3908,11 @@
       <c r="C191">
         <v>27.2408</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191">
+        <v>26.515799999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -3346,8 +3922,11 @@
       <c r="C192">
         <v>7.2452100000000002</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192">
+        <v>7.24681</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -3357,8 +3936,11 @@
       <c r="C193">
         <v>3.6432500000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193">
+        <v>3.60426</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -3368,8 +3950,11 @@
       <c r="C194">
         <v>2.5868899999999999</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194">
+        <v>2.5520200000000002</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -3379,8 +3964,11 @@
       <c r="C195">
         <v>2.9933999999999998</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195">
+        <v>2.9545699999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -3390,8 +3978,11 @@
       <c r="C196">
         <v>3.6890299999999998</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196">
+        <v>3.65951</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -3401,8 +3992,11 @@
       <c r="C197">
         <v>3.4126799999999999</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197">
+        <v>3.36572</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -3412,8 +4006,11 @@
       <c r="C198">
         <v>2.2292000000000001</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198">
+        <v>2.2051799999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -3423,8 +4020,11 @@
       <c r="C199">
         <v>7.5115299999999996</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199">
+        <v>7.4545000000000003</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -3434,8 +4034,11 @@
       <c r="C200">
         <v>3.41608</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200">
+        <v>3.39208</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -3445,8 +4048,11 @@
       <c r="C201">
         <v>2.8449</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201">
+        <v>2.8134100000000002</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3456,8 +4062,11 @@
       <c r="C202">
         <v>24.673999999999999</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202">
+        <v>24.0059</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -3467,8 +4076,11 @@
       <c r="C203">
         <v>2.7590300000000001</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203">
+        <v>2.7611400000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -3478,8 +4090,11 @@
       <c r="C204">
         <v>3.8268200000000001</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204">
+        <v>3.7993800000000002</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3489,8 +4104,11 @@
       <c r="C205">
         <v>1.9801</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205">
+        <v>1.95902</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3500,8 +4118,11 @@
       <c r="C206">
         <v>3.6562999999999999</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206">
+        <v>3.6311399999999998</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3511,8 +4132,11 @@
       <c r="C207">
         <v>2.1384799999999999</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207">
+        <v>2.1124900000000002</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3522,8 +4146,11 @@
       <c r="C208">
         <v>2.0411800000000002</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208">
+        <v>2.0237400000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3533,8 +4160,11 @@
       <c r="C209">
         <v>3.1840099999999998</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209">
+        <v>3.1656300000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3544,8 +4174,11 @@
       <c r="C210">
         <v>1.6666799999999999</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D210">
+        <v>1.6426499999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3555,8 +4188,11 @@
       <c r="C211">
         <v>7.3806900000000004</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D211">
+        <v>7.3364799999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -3566,8 +4202,11 @@
       <c r="C212">
         <v>1.7861100000000001</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D212">
+        <v>1.76657</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -3577,8 +4216,11 @@
       <c r="C213">
         <v>25.298999999999999</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D213">
+        <v>24.5654</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -3588,8 +4230,11 @@
       <c r="C214">
         <v>946.98299999999995</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D214">
+        <v>937.77099999999996</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -3599,8 +4244,11 @@
       <c r="C215">
         <v>67.205500000000001</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D215">
+        <v>66.577100000000002</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -3610,8 +4258,11 @@
       <c r="C216">
         <v>26.1327</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216">
+        <v>25.4023</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -3621,8 +4272,11 @@
       <c r="C217">
         <v>26.182500000000001</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D217">
+        <v>25.433399999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3632,8 +4286,11 @@
       <c r="C218">
         <v>46.428699999999999</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D218">
+        <v>44.950099999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -3643,8 +4300,11 @@
       <c r="C219">
         <v>14.053900000000001</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D219">
+        <v>13.7075</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -3654,8 +4314,11 @@
       <c r="C220">
         <v>24.988299999999999</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D220">
+        <v>24.323899999999998</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3665,8 +4328,11 @@
       <c r="C221">
         <v>23.224799999999998</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D221">
+        <v>22.655000000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -3676,8 +4342,11 @@
       <c r="C222">
         <v>23.155999999999999</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D222">
+        <v>22.593499999999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -3687,8 +4356,11 @@
       <c r="C223">
         <v>28.0624</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D223">
+        <v>27.274799999999999</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -3698,8 +4370,11 @@
       <c r="C224">
         <v>25.4422</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D224">
+        <v>24.745999999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -3709,8 +4384,11 @@
       <c r="C225">
         <v>38.914200000000001</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D225">
+        <v>37.972000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -3720,8 +4398,11 @@
       <c r="C226">
         <v>25.558800000000002</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D226">
+        <v>24.8551</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -3731,8 +4412,11 @@
       <c r="C227">
         <v>25.967600000000001</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D227">
+        <v>24.6341</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -3742,8 +4426,11 @@
       <c r="C228">
         <v>27.3094</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D228">
+        <v>26.354500000000002</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -3753,8 +4440,11 @@
       <c r="C229">
         <v>13.677099999999999</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D229">
+        <v>13.8241</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -3764,8 +4454,11 @@
       <c r="C230">
         <v>55.325299999999999</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D230">
+        <v>55.357599999999998</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -3775,8 +4468,11 @@
       <c r="C231">
         <v>56.467500000000001</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D231">
+        <v>55.8504</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -3786,8 +4482,11 @@
       <c r="C232">
         <v>26.5258</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D232">
+        <v>26.183800000000002</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -3797,8 +4496,11 @@
       <c r="C233">
         <v>6.8350200000000001</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D233">
+        <v>6.8863799999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -3808,8 +4510,11 @@
       <c r="C234">
         <v>1.8347800000000001</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D234">
+        <v>1.83087</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -3819,8 +4524,11 @@
       <c r="C235">
         <v>1.5651600000000001</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D235">
+        <v>1.56477</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -3830,8 +4538,11 @@
       <c r="C236">
         <v>5.16927</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D236">
+        <v>5.2576499999999999</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -3841,8 +4552,11 @@
       <c r="C237">
         <v>24.651399999999999</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D237">
+        <v>24.492000000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -3852,8 +4566,11 @@
       <c r="C238">
         <v>3.1613899999999999</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D238">
+        <v>3.2837299999999998</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -3863,8 +4580,11 @@
       <c r="C239">
         <v>3.6173099999999998</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D239">
+        <v>3.7015699999999998</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -3874,8 +4594,11 @@
       <c r="C240">
         <v>3.4849700000000001</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D240">
+        <v>3.46041</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -3885,8 +4608,11 @@
       <c r="C241">
         <v>1.90147</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D241">
+        <v>1.867</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -3896,8 +4622,11 @@
       <c r="C242">
         <v>1.83883</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D242">
+        <v>1.7947200000000001</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -3907,8 +4636,11 @@
       <c r="C243">
         <v>3.7158099999999998</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D243">
+        <v>3.5498799999999999</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -3918,8 +4650,11 @@
       <c r="C244">
         <v>5.2947899999999999</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D244">
+        <v>4.9204600000000003</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -3929,8 +4664,11 @@
       <c r="C245">
         <v>5.2603</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D245">
+        <v>4.9609399999999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -3940,8 +4678,11 @@
       <c r="C246">
         <v>3.3912399999999998</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D246">
+        <v>3.2684000000000002</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -3951,8 +4692,11 @@
       <c r="C247">
         <v>3.0268299999999999</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D247">
+        <v>3.0028199999999998</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -3962,8 +4706,11 @@
       <c r="C248">
         <v>24.558299999999999</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D248">
+        <v>23.942699999999999</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -3973,8 +4720,11 @@
       <c r="C249">
         <v>5.8661500000000002</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D249">
+        <v>5.9501900000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -3984,8 +4734,11 @@
       <c r="C250">
         <v>1.8889</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>1.88375</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -3995,8 +4748,11 @@
       <c r="C251">
         <v>7.4298200000000003</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D251">
+        <v>7.03512</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -4006,8 +4762,11 @@
       <c r="C252">
         <v>1.9285699999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D252">
+        <v>1.86273</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -4017,8 +4776,11 @@
       <c r="C253">
         <v>3.3304299999999998</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D253">
+        <v>3.1762800000000002</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -4028,8 +4790,11 @@
       <c r="C254">
         <v>32.994999999999997</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D254">
+        <v>31.100200000000001</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -4039,8 +4804,11 @@
       <c r="C255">
         <v>5.5341199999999997</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D255">
+        <v>3.9602499999999998</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -4050,8 +4818,11 @@
       <c r="C256">
         <v>2.6537500000000001</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D256">
+        <v>2.7768000000000002</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -4061,8 +4832,11 @@
       <c r="C257">
         <v>2.7566199999999998</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257">
+        <v>3.0318000000000001</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -4072,8 +4846,11 @@
       <c r="C258">
         <v>7.2299199999999999</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D258">
+        <v>7.2246199999999998</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -4083,8 +4860,11 @@
       <c r="C259">
         <v>50.202800000000003</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D259">
+        <v>46.543300000000002</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -4094,8 +4874,11 @@
       <c r="C260">
         <v>5.6497999999999999</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D260">
+        <v>5.5282299999999998</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -4105,8 +4888,11 @@
       <c r="C261">
         <v>2.8104</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D261">
+        <v>2.7486799999999998</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -4116,8 +4902,11 @@
       <c r="C262">
         <v>2.54637</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D262">
+        <v>2.4890099999999999</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -4127,8 +4916,11 @@
       <c r="C263">
         <v>1.75559</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D263">
+        <v>1.7404999999999999</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -4138,8 +4930,11 @@
       <c r="C264">
         <v>4.9632699999999996</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D264">
+        <v>4.9089099999999997</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -4149,8 +4944,11 @@
       <c r="C265">
         <v>3.19049</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D265">
+        <v>3.1505100000000001</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -4160,8 +4958,11 @@
       <c r="C266">
         <v>2.8988999999999998</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D266">
+        <v>2.8910999999999998</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -4171,8 +4972,11 @@
       <c r="C267">
         <v>1.9989699999999999</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D267">
+        <v>1.97611</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -4182,8 +4986,11 @@
       <c r="C268">
         <v>3.4180899999999999</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D268">
+        <v>3.3940299999999999</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -4193,8 +5000,11 @@
       <c r="C269">
         <v>5.9312899999999997</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D269">
+        <v>5.9146799999999997</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -4204,8 +5014,11 @@
       <c r="C270">
         <v>24.663900000000002</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D270">
+        <v>24.3279</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -4215,8 +5028,11 @@
       <c r="C271">
         <v>6.6098600000000003</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D271">
+        <v>7.11822</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -4226,8 +5042,11 @@
       <c r="C272">
         <v>2.97241</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272">
+        <v>3.30782</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -4237,8 +5056,11 @@
       <c r="C273">
         <v>2.9401700000000002</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273">
+        <v>3.5026700000000002</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -4248,8 +5070,11 @@
       <c r="C274">
         <v>2.4914700000000001</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D274">
+        <v>3.1831399999999999</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -4259,8 +5084,11 @@
       <c r="C275">
         <v>3.07254</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D275">
+        <v>3.4848499999999998</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -4270,8 +5098,11 @@
       <c r="C276">
         <v>4.1697499999999996</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D276">
+        <v>4.8930499999999997</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -4281,8 +5112,11 @@
       <c r="C277">
         <v>3.3603499999999999</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D277">
+        <v>3.7515900000000002</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -4292,8 +5126,11 @@
       <c r="C278">
         <v>2.9581</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D278">
+        <v>3.3631099999999998</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -4303,8 +5140,11 @@
       <c r="C279">
         <v>4.1511199999999997</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D279">
+        <v>4.4611999999999998</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -4314,8 +5154,11 @@
       <c r="C280">
         <v>2.8483499999999999</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D280">
+        <v>2.83826</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -4325,8 +5168,11 @@
       <c r="C281">
         <v>24.573</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D281">
+        <v>24.2654</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -4336,8 +5182,11 @@
       <c r="C282">
         <v>3.22898</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D282">
+        <v>3.2206999999999999</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -4347,8 +5196,11 @@
       <c r="C283">
         <v>3.24865</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D283">
+        <v>3.2284600000000001</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -4358,8 +5210,11 @@
       <c r="C284">
         <v>2.51912</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D284">
+        <v>2.5009899999999998</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -4369,8 +5224,11 @@
       <c r="C285">
         <v>2.4266899999999998</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D285">
+        <v>2.3863799999999999</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -4380,8 +5238,11 @@
       <c r="C286">
         <v>3.4679899999999999</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D286">
+        <v>3.4406300000000001</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -4391,8 +5252,11 @@
       <c r="C287">
         <v>2.1819500000000001</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D287">
+        <v>2.1699799999999998</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -4402,8 +5266,11 @@
       <c r="C288">
         <v>3.09354</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288">
+        <v>3.0616099999999999</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -4413,8 +5280,11 @@
       <c r="C289">
         <v>2.67252</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289">
+        <v>2.6474000000000002</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -4424,8 +5294,11 @@
       <c r="C290">
         <v>4.2746599999999999</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290">
+        <v>4.2421300000000004</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -4435,13 +5308,19 @@
       <c r="C291">
         <v>2.5573700000000001</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D291">
+        <v>2.5208499999999998</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>291</v>
       </c>
       <c r="C292" t="s">
         <v>292</v>
+      </c>
+      <c r="D292" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove some useless code
</commit_message>
<xml_diff>
--- a/app/result.xlsx
+++ b/app/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QOC_Src\MeshSimplication.Android\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QOC\MeshSimplification-Mobile\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC50B5F-1B2A-4772-8C6F-70137ABF3507}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BFB764-D1AD-472E-B05B-2DBB5E59266D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1875" windowWidth="28095" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
   <si>
     <t>mesh0</t>
   </si>
@@ -936,6 +938,9 @@
   </si>
   <si>
     <t>Vector Neighbors</t>
+  </si>
+  <si>
+    <t>Remove some useless code</t>
   </si>
 </sst>
 </file>
@@ -16944,10 +16949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K292"/>
+  <dimension ref="A1:L292"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E271" workbookViewId="0">
-      <selection activeCell="K293" sqref="K293"/>
+      <selection activeCell="L293" sqref="L293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16962,9 +16967,10 @@
     <col min="9" max="9" width="36.28515625" customWidth="1"/>
     <col min="10" max="10" width="32.140625" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16998,8 +17004,11 @@
       <c r="K1">
         <v>20.648499999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1">
+        <v>19.431899999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -17033,8 +17042,11 @@
       <c r="K2">
         <v>19.551500000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>18.1708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -17068,8 +17080,11 @@
       <c r="K3">
         <v>18.732099999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>17.616900000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -17103,8 +17118,11 @@
       <c r="K4">
         <v>3.95764</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>3.9021300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -17138,8 +17156,11 @@
       <c r="K5">
         <v>2.4885700000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>2.4193699999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -17173,8 +17194,11 @@
       <c r="K6">
         <v>2.0930900000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>2.0263200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -17208,8 +17232,11 @@
       <c r="K7">
         <v>1.5454699999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>1.52044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -17243,8 +17270,11 @@
       <c r="K8">
         <v>3.2878799999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>3.2593899999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -17278,8 +17308,11 @@
       <c r="K9">
         <v>3.2105199999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>3.0947200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -17313,8 +17346,11 @@
       <c r="K10">
         <v>1.88191</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>1.8559000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -17348,8 +17384,11 @@
       <c r="K11">
         <v>3.4393500000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>3.3941300000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -17383,8 +17422,11 @@
       <c r="K12">
         <v>1.5442499999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>1.5288900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -17418,8 +17460,11 @@
       <c r="K13">
         <v>4.2563399999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>3.9937100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -17453,8 +17498,11 @@
       <c r="K14">
         <v>31.3901</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>29.472799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -17488,8 +17536,11 @@
       <c r="K15">
         <v>3.7507799999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>3.6471399999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -17523,8 +17574,11 @@
       <c r="K16">
         <v>1.93794</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>1.9044000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -17558,8 +17612,11 @@
       <c r="K17">
         <v>1.87924</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>1.85118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -17593,8 +17650,11 @@
       <c r="K18">
         <v>1.83785</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>1.8063400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -17628,8 +17688,11 @@
       <c r="K19">
         <v>2.03843</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>1.99444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -17663,8 +17726,11 @@
       <c r="K20">
         <v>3.2170299999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>3.1205699999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -17698,8 +17764,11 @@
       <c r="K21">
         <v>2.9918999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>2.98881</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -17733,8 +17802,11 @@
       <c r="K22">
         <v>1.4713400000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1.4705999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -17768,8 +17840,11 @@
       <c r="K23">
         <v>2.4145400000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>2.3296999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -17803,8 +17878,11 @@
       <c r="K24">
         <v>2.9394100000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>2.8467699999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -17838,8 +17916,11 @@
       <c r="K25">
         <v>34.317799999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>32.456699999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -17873,8 +17954,11 @@
       <c r="K26">
         <v>2.2997700000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>2.25617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -17908,8 +17992,11 @@
       <c r="K27">
         <v>3.97153</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>3.87995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -17943,8 +18030,11 @@
       <c r="K28">
         <v>1.5877600000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>1.5652999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -17978,8 +18068,11 @@
       <c r="K29">
         <v>1.9959899999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>1.9605699999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -18013,8 +18106,11 @@
       <c r="K30">
         <v>2.1341000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>2.07803</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -18048,8 +18144,11 @@
       <c r="K31">
         <v>3.2328100000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>3.1968000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -18083,8 +18182,11 @@
       <c r="K32">
         <v>2.6283599999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>2.5554600000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -18118,8 +18220,11 @@
       <c r="K33">
         <v>1.97288</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>1.93384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -18153,8 +18258,11 @@
       <c r="K34">
         <v>1.7127699999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>1.68641</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -18188,8 +18296,11 @@
       <c r="K35">
         <v>4.57559</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>4.4061500000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -18223,8 +18334,11 @@
       <c r="K36">
         <v>18.441099999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>17.3369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -18258,8 +18372,11 @@
       <c r="K37">
         <v>3.2056200000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>3.0843699999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -18293,8 +18410,11 @@
       <c r="K38">
         <v>2.85589</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>2.78186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -18328,8 +18448,11 @@
       <c r="K39">
         <v>1.69638</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>1.67685</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -18363,8 +18486,11 @@
       <c r="K40">
         <v>2.8561100000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>2.7570899999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -18398,8 +18524,11 @@
       <c r="K41">
         <v>2.12588</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>2.0746199999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -18433,8 +18562,11 @@
       <c r="K42">
         <v>2.3138000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>2.2567499999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -18468,8 +18600,11 @@
       <c r="K43">
         <v>2.2128700000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>2.16873</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -18503,8 +18638,11 @@
       <c r="K44">
         <v>2.2616000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>2.2003499999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -18538,8 +18676,11 @@
       <c r="K45">
         <v>1.61554</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>1.5862700000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -18573,8 +18714,11 @@
       <c r="K46">
         <v>2.3356499999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>2.28308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -18608,8 +18752,11 @@
       <c r="K47">
         <v>20.505700000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>19.319299999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -18643,8 +18790,11 @@
       <c r="K48">
         <v>1.9949699999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>1.96776</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -18678,8 +18828,11 @@
       <c r="K49">
         <v>2.5747499999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>2.5141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -18713,8 +18866,11 @@
       <c r="K50">
         <v>1.7364299999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>1.70625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -18748,8 +18904,11 @@
       <c r="K51">
         <v>3.23746</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>3.1915900000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -18783,8 +18942,11 @@
       <c r="K52">
         <v>3.4329900000000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>3.2984100000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -18818,8 +18980,11 @@
       <c r="K53">
         <v>2.6388400000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>2.56941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -18853,8 +19018,11 @@
       <c r="K54">
         <v>1.6871700000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>1.6635899999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -18888,8 +19056,11 @@
       <c r="K55">
         <v>2.37534</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>2.29088</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -18923,8 +19094,11 @@
       <c r="K56">
         <v>2.7225799999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>2.6329099999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -18958,8 +19132,11 @@
       <c r="K57">
         <v>2.1947899999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>2.14418</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -18993,8 +19170,11 @@
       <c r="K58">
         <v>18.266300000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>17.164400000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -19028,8 +19208,11 @@
       <c r="K59">
         <v>3.3875500000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>3.3637800000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -19063,8 +19246,11 @@
       <c r="K60">
         <v>1.7456</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>1.7248000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -19098,8 +19284,11 @@
       <c r="K61">
         <v>1.6984300000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>1.66734</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -19133,8 +19322,11 @@
       <c r="K62">
         <v>3.3829899999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>3.16133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -19168,8 +19360,11 @@
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -19203,8 +19398,11 @@
       <c r="K64">
         <v>2.7856900000000002</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>2.6826599999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -19238,8 +19436,11 @@
       <c r="K65">
         <v>4.8311599999999997</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>4.61937</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -19273,8 +19474,11 @@
       <c r="K66">
         <v>9.4176400000000005</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>8.8847500000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -19308,8 +19512,11 @@
       <c r="K67">
         <v>2.2109299999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>2.15815</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -19343,8 +19550,11 @@
       <c r="K68">
         <v>2.07613</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>2.0424600000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -19378,8 +19588,11 @@
       <c r="K69">
         <v>20.4255</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <v>19.234000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -19413,8 +19626,11 @@
       <c r="K70">
         <v>2.19184</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <v>2.13279</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -19448,8 +19664,11 @@
       <c r="K71">
         <v>1.58474</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>1.5789</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -19483,8 +19702,11 @@
       <c r="K72">
         <v>1.72722</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>1.71574</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -19518,8 +19740,11 @@
       <c r="K73">
         <v>3.16248</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>3.12371</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -19553,8 +19778,11 @@
       <c r="K74">
         <v>1.57467</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <v>1.5626100000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -19588,8 +19816,11 @@
       <c r="K75">
         <v>3.2642500000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>3.2479</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -19623,8 +19854,11 @@
       <c r="K76">
         <v>3.0050400000000002</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>2.9997600000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -19658,8 +19892,11 @@
       <c r="K77">
         <v>2.7031900000000002</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>2.6389800000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -19693,8 +19930,11 @@
       <c r="K78">
         <v>1.93353</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>1.88052</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -19728,8 +19968,11 @@
       <c r="K79">
         <v>3.1880099999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>3.1662300000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -19763,8 +20006,11 @@
       <c r="K80">
         <v>18.215</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>17.1175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -19798,8 +20044,11 @@
       <c r="K81">
         <v>1.95946</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>1.9275599999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -19833,8 +20082,11 @@
       <c r="K82">
         <v>1.8950499999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>1.87931</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -19868,8 +20120,11 @@
       <c r="K83">
         <v>2.49071</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83">
+        <v>2.3993899999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -19903,8 +20158,11 @@
       <c r="K84">
         <v>4.6604200000000002</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>4.4831399999999997</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -19938,8 +20196,11 @@
       <c r="K85">
         <v>2.9528500000000002</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>2.8646799999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -19973,8 +20234,11 @@
       <c r="K86">
         <v>2.6242899999999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>2.4827300000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -20008,8 +20272,11 @@
       <c r="K87">
         <v>2.9789599999999998</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>2.95078</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -20043,8 +20310,11 @@
       <c r="K88">
         <v>2.93262</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>2.9337599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -20078,8 +20348,11 @@
       <c r="K89">
         <v>1.6194999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>1.6059099999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -20113,8 +20386,11 @@
       <c r="K90">
         <v>2.9325199999999998</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>2.92909</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -20148,8 +20424,11 @@
       <c r="K91">
         <v>20.372499999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>19.198799999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -20183,8 +20462,11 @@
       <c r="K92">
         <v>2.1103100000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <v>2.0503499999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -20218,8 +20500,11 @@
       <c r="K93">
         <v>1.7806500000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <v>1.7637799999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -20253,8 +20538,11 @@
       <c r="K94">
         <v>1.66523</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94">
+        <v>1.6487099999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -20288,8 +20576,11 @@
       <c r="K95">
         <v>3.5535700000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <v>3.4836200000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -20323,8 +20614,11 @@
       <c r="K96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -20358,8 +20652,11 @@
       <c r="K97">
         <v>3.0149499999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97">
+        <v>2.9998200000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -20393,8 +20690,11 @@
       <c r="K98">
         <v>3.0840900000000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98">
+        <v>3.0857299999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -20428,8 +20728,11 @@
       <c r="K99">
         <v>3.0406900000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99">
+        <v>3.0373899999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -20463,8 +20766,11 @@
       <c r="K100">
         <v>3.9136600000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100">
+        <v>3.7796699999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -20498,8 +20804,11 @@
       <c r="K101">
         <v>1.7934300000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101">
+        <v>1.7672300000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -20533,8 +20842,11 @@
       <c r="K102">
         <v>18.4558</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102">
+        <v>17.361799999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -20568,8 +20880,11 @@
       <c r="K103">
         <v>4.0510999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103">
+        <v>3.8849800000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -20603,8 +20918,11 @@
       <c r="K104">
         <v>2.2250100000000002</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104">
+        <v>2.1930999999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -20638,8 +20956,11 @@
       <c r="K105">
         <v>2.1833100000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105">
+        <v>2.12778</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -20673,8 +20994,11 @@
       <c r="K106">
         <v>1.6492</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106">
+        <v>1.6262300000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -20708,8 +21032,11 @@
       <c r="K107">
         <v>2.1038000000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107">
+        <v>2.0605000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -20743,8 +21070,11 @@
       <c r="K108">
         <v>2.94895</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108">
+        <v>2.94346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -20778,8 +21108,11 @@
       <c r="K109">
         <v>1.5008900000000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109">
+        <v>1.50865</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -20813,8 +21146,11 @@
       <c r="K110">
         <v>1.7745200000000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110">
+        <v>1.75143</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -20848,8 +21184,11 @@
       <c r="K111">
         <v>3.0225</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111">
+        <v>2.99973</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -20883,8 +21222,11 @@
       <c r="K112">
         <v>2.92265</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112">
+        <v>2.9255300000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -20918,8 +21260,11 @@
       <c r="K113">
         <v>18.284199999999998</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113">
+        <v>17.204699999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -20953,8 +21298,11 @@
       <c r="K114">
         <v>18.802900000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114">
+        <v>17.719000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -20988,8 +21336,11 @@
       <c r="K115">
         <v>3.3561200000000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115">
+        <v>3.3180499999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -21023,8 +21374,11 @@
       <c r="K116">
         <v>2.3805000000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116">
+        <v>2.31671</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -21058,8 +21412,11 @@
       <c r="K117">
         <v>3.0701999999999998</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117">
+        <v>3.0358100000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -21093,8 +21450,11 @@
       <c r="K118">
         <v>2.1259899999999998</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118">
+        <v>2.0699700000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -21128,8 +21488,11 @@
       <c r="K119">
         <v>1.7485200000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119">
+        <v>1.7095</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -21163,8 +21526,11 @@
       <c r="K120">
         <v>1.68079</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120">
+        <v>1.67774</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -21198,8 +21564,11 @@
       <c r="K121">
         <v>3.07497</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121">
+        <v>2.9838200000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -21233,8 +21602,11 @@
       <c r="K122">
         <v>4.32761</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122">
+        <v>4.1216999999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -21268,8 +21640,11 @@
       <c r="K123">
         <v>9.6759799999999991</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123">
+        <v>8.8770799999999994</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -21303,8 +21678,11 @@
       <c r="K124">
         <v>2.9090400000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124">
+        <v>2.83508</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -21338,8 +21716,11 @@
       <c r="K125">
         <v>20.5717</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125">
+        <v>19.343699999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -21373,8 +21754,11 @@
       <c r="K126">
         <v>6.5276300000000003</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126">
+        <v>6.1675800000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -21408,8 +21792,11 @@
       <c r="K127">
         <v>3.1975500000000001</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127">
+        <v>3.1681499999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -21443,8 +21830,11 @@
       <c r="K128">
         <v>3.1800700000000002</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L128">
+        <v>3.08772</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -21478,8 +21868,11 @@
       <c r="K129">
         <v>3.0634999999999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L129">
+        <v>2.9885299999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -21513,8 +21906,11 @@
       <c r="K130">
         <v>1.7608200000000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130">
+        <v>1.7380500000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -21548,8 +21944,11 @@
       <c r="K131">
         <v>10.0046</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131">
+        <v>9.3874999999999993</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -21583,8 +21982,11 @@
       <c r="K132">
         <v>2.4003999999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132">
+        <v>2.3379799999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -21618,8 +22020,11 @@
       <c r="K133">
         <v>3.5739200000000002</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133">
+        <v>3.44374</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -21653,8 +22058,11 @@
       <c r="K134">
         <v>4.3984500000000004</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134">
+        <v>4.2175000000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -21688,8 +22096,11 @@
       <c r="K135">
         <v>5.3123699999999996</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135">
+        <v>5.1078200000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -21723,8 +22134,11 @@
       <c r="K136">
         <v>11.341799999999999</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L136">
+        <v>10.695600000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -21758,8 +22172,11 @@
       <c r="K137">
         <v>8.6549200000000006</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137">
+        <v>8.2076600000000006</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -21793,8 +22210,11 @@
       <c r="K138">
         <v>4.85663</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138">
+        <v>4.6393800000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -21828,8 +22248,11 @@
       <c r="K139">
         <v>25.903099999999998</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139">
+        <v>24.298300000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -21863,8 +22286,11 @@
       <c r="K140">
         <v>24.6557</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140">
+        <v>23.264500000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -21898,8 +22324,11 @@
       <c r="K141">
         <v>3.4919799999999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L141">
+        <v>3.3595100000000002</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -21933,8 +22362,11 @@
       <c r="K142">
         <v>5.2617799999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L142">
+        <v>5.0315000000000003</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -21968,8 +22400,11 @@
       <c r="K143">
         <v>5.0010599999999998</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L143">
+        <v>4.7852100000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -22003,8 +22438,11 @@
       <c r="K144">
         <v>1.9624200000000001</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L144">
+        <v>1.93319</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -22038,8 +22476,11 @@
       <c r="K145">
         <v>4.2207400000000002</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145">
+        <v>4.0133099999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -22073,8 +22514,11 @@
       <c r="K146">
         <v>2.39628</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L146">
+        <v>2.3414299999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -22108,8 +22552,11 @@
       <c r="K147">
         <v>20.426500000000001</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L147">
+        <v>19.235600000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -22143,8 +22590,11 @@
       <c r="K148">
         <v>7.0059800000000001</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L148">
+        <v>6.6599399999999997</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -22178,8 +22628,11 @@
       <c r="K149">
         <v>5.9464399999999999</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L149">
+        <v>5.7073</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -22213,8 +22666,11 @@
       <c r="K150">
         <v>9.4525000000000006</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L150">
+        <v>8.9768500000000007</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -22248,8 +22704,11 @@
       <c r="K151">
         <v>14.2402</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L151">
+        <v>13.3606</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -22283,8 +22742,11 @@
       <c r="K152">
         <v>2.29983</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L152">
+        <v>2.2492000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -22318,8 +22780,11 @@
       <c r="K153">
         <v>3.6659799999999998</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L153">
+        <v>3.5232299999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -22353,8 +22818,11 @@
       <c r="K154">
         <v>4.12927</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L154">
+        <v>3.99038</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -22388,8 +22856,11 @@
       <c r="K155">
         <v>5.1364799999999997</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L155">
+        <v>4.9405900000000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -22423,8 +22894,11 @@
       <c r="K156">
         <v>6.6255899999999999</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156">
+        <v>6.3319299999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -22458,8 +22932,11 @@
       <c r="K157">
         <v>15.126200000000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L157">
+        <v>14.3741</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -22493,8 +22970,11 @@
       <c r="K158">
         <v>20.641200000000001</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L158">
+        <v>19.484500000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -22528,8 +23008,11 @@
       <c r="K159">
         <v>4.8124599999999997</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L159">
+        <v>4.6041400000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -22563,8 +23046,11 @@
       <c r="K160">
         <v>2.4790299999999998</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L160">
+        <v>2.4238499999999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -22598,8 +23084,11 @@
       <c r="K161">
         <v>3.2710400000000002</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L161">
+        <v>3.1610100000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -22633,8 +23122,11 @@
       <c r="K162">
         <v>6.9188999999999998</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L162">
+        <v>6.6148199999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -22668,8 +23160,11 @@
       <c r="K163">
         <v>6.1485200000000004</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L163">
+        <v>5.85487</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -22703,8 +23198,11 @@
       <c r="K164">
         <v>2.20689</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L164">
+        <v>2.16147</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -22738,8 +23236,11 @@
       <c r="K165">
         <v>4.2887300000000002</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L165">
+        <v>4.1164399999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -22773,8 +23274,11 @@
       <c r="K166">
         <v>4.7427200000000003</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L166">
+        <v>4.56576</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -22808,8 +23312,11 @@
       <c r="K167">
         <v>5.38605</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L167">
+        <v>5.1493399999999996</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -22843,8 +23350,11 @@
       <c r="K168">
         <v>4.43147</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L168">
+        <v>4.25943</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -22878,8 +23388,11 @@
       <c r="K169">
         <v>31.4968</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L169">
+        <v>29.587399999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -22913,8 +23426,11 @@
       <c r="K170">
         <v>6.3552499999999998</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L170">
+        <v>6.0519800000000004</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -22948,8 +23464,11 @@
       <c r="K171">
         <v>3.80002</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L171">
+        <v>3.7387600000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -22983,8 +23502,11 @@
       <c r="K172">
         <v>2.09579</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L172">
+        <v>2.0560900000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -23018,8 +23540,11 @@
       <c r="K173">
         <v>2.4926300000000001</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L173">
+        <v>2.4132199999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -23053,8 +23578,11 @@
       <c r="K174">
         <v>2.9509599999999998</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L174">
+        <v>2.8227000000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -23088,8 +23616,11 @@
       <c r="K175">
         <v>2.1090100000000001</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L175">
+        <v>2.06657</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -23123,8 +23654,11 @@
       <c r="K176">
         <v>4.1799099999999996</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L176">
+        <v>4.0359299999999996</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -23158,8 +23692,11 @@
       <c r="K177">
         <v>4.0691699999999997</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L177">
+        <v>3.88619</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -23193,8 +23730,11 @@
       <c r="K178">
         <v>3.4268100000000001</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L178">
+        <v>3.3156500000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -23228,8 +23768,11 @@
       <c r="K179">
         <v>4.8885699999999996</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L179">
+        <v>4.6794700000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -23263,8 +23806,11 @@
       <c r="K180">
         <v>20.559899999999999</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L180">
+        <v>19.3706</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -23298,8 +23844,11 @@
       <c r="K181">
         <v>3.1474899999999999</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L181">
+        <v>3.0338099999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -23333,8 +23882,11 @@
       <c r="K182">
         <v>6.95085</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L182">
+        <v>6.6486099999999997</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -23368,8 +23920,11 @@
       <c r="K183">
         <v>2.6293700000000002</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L183">
+        <v>2.57016</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -23403,8 +23958,11 @@
       <c r="K184">
         <v>3.2685599999999999</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L184">
+        <v>3.23624</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -23438,8 +23996,11 @@
       <c r="K185">
         <v>2.2792400000000002</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L185">
+        <v>2.2289099999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -23473,8 +24034,11 @@
       <c r="K186">
         <v>4.1349999999999998</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L186">
+        <v>3.9518900000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -23508,8 +24072,11 @@
       <c r="K187">
         <v>1.92624</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L187">
+        <v>1.8925000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -23543,8 +24110,11 @@
       <c r="K188">
         <v>4.9359000000000002</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L188">
+        <v>4.75197</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -23578,8 +24148,11 @@
       <c r="K189">
         <v>1.56915</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L189">
+        <v>1.5580700000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -23613,8 +24186,11 @@
       <c r="K190">
         <v>1.8284</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L190">
+        <v>1.7926299999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -23648,8 +24224,11 @@
       <c r="K191">
         <v>20.4404</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L191">
+        <v>19.244599999999998</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -23683,8 +24262,11 @@
       <c r="K192">
         <v>5.5254399999999997</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L192">
+        <v>5.2834099999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -23718,8 +24300,11 @@
       <c r="K193">
         <v>2.9416000000000002</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L193">
+        <v>2.8450600000000001</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -23753,8 +24338,11 @@
       <c r="K194">
         <v>2.22424</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L194">
+        <v>2.1722999999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -23788,8 +24376,11 @@
       <c r="K195">
         <v>2.2326999999999999</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L195">
+        <v>2.16845</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -23823,8 +24414,11 @@
       <c r="K196">
         <v>3.17822</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L196">
+        <v>3.0969699999999998</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -23858,8 +24452,11 @@
       <c r="K197">
         <v>2.7717200000000002</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L197">
+        <v>2.6851600000000002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -23893,8 +24490,11 @@
       <c r="K198">
         <v>1.9706399999999999</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L198">
+        <v>1.92852</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -23928,8 +24528,11 @@
       <c r="K199">
         <v>6.0065200000000001</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L199">
+        <v>5.7403599999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -23963,8 +24566,11 @@
       <c r="K200">
         <v>2.7808799999999998</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L200">
+        <v>2.6906500000000002</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -23998,8 +24604,11 @@
       <c r="K201">
         <v>2.42875</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L201">
+        <v>2.3557199999999998</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -24033,8 +24642,11 @@
       <c r="K202">
         <v>18.447500000000002</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L202">
+        <v>17.353100000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -24068,8 +24680,11 @@
       <c r="K203">
         <v>2.2171500000000002</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L203">
+        <v>2.15788</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -24103,8 +24718,11 @@
       <c r="K204">
         <v>3.1257700000000002</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L204">
+        <v>3.0249299999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -24138,8 +24756,11 @@
       <c r="K205">
         <v>1.7990699999999999</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L205">
+        <v>1.7763599999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -24173,8 +24794,11 @@
       <c r="K206">
         <v>3.1695500000000001</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L206">
+        <v>3.0802399999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -24208,8 +24832,11 @@
       <c r="K207">
         <v>1.90907</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L207">
+        <v>1.8756200000000001</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -24243,8 +24870,11 @@
       <c r="K208">
         <v>1.8714500000000001</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L208">
+        <v>1.8431500000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -24278,8 +24908,11 @@
       <c r="K209">
         <v>2.7538</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L209">
+        <v>2.6946500000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -24313,8 +24946,11 @@
       <c r="K210">
         <v>1.5842799999999999</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L210">
+        <v>1.56517</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -24348,8 +24984,11 @@
       <c r="K211">
         <v>5.7303600000000001</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L211">
+        <v>5.4619299999999997</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -24383,8 +25022,11 @@
       <c r="K212">
         <v>1.6479699999999999</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L212">
+        <v>1.63771</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -24418,8 +25060,11 @@
       <c r="K213">
         <v>18.834099999999999</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L213">
+        <v>17.693899999999999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -24453,8 +25098,11 @@
       <c r="K214">
         <v>550.28599999999994</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L214">
+        <v>507.85899999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -24488,8 +25136,11 @@
       <c r="K215">
         <v>31.529800000000002</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L215">
+        <v>28.508500000000002</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -24523,8 +25174,11 @@
       <c r="K216">
         <v>19.292400000000001</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L216">
+        <v>18.141100000000002</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -24558,8 +25212,11 @@
       <c r="K217">
         <v>19.3095</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L217">
+        <v>18.160499999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -24593,8 +25250,11 @@
       <c r="K218">
         <v>34.986199999999997</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L218">
+        <v>33.0398</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -24628,8 +25288,11 @@
       <c r="K219">
         <v>10.0617</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L219">
+        <v>9.4524600000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -24663,8 +25326,11 @@
       <c r="K220">
         <v>18.5077</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L220">
+        <v>17.4316</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -24698,8 +25364,11 @@
       <c r="K221">
         <v>17.036999999999999</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L221">
+        <v>16.0259</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -24733,8 +25402,11 @@
       <c r="K222">
         <v>16.970700000000001</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L222">
+        <v>15.9756</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -24768,8 +25440,11 @@
       <c r="K223">
         <v>20.835599999999999</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L223">
+        <v>19.6388</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -24803,8 +25478,11 @@
       <c r="K224">
         <v>18.732399999999998</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L224">
+        <v>17.626899999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -24838,8 +25516,11 @@
       <c r="K225">
         <v>29.024999999999999</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L225">
+        <v>27.377300000000002</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -24873,8 +25554,11 @@
       <c r="K226">
         <v>18.731100000000001</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L226">
+        <v>17.6342</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -24908,8 +25592,11 @@
       <c r="K227">
         <v>18.704799999999999</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L227">
+        <v>17.616199999999999</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -24943,8 +25630,11 @@
       <c r="K228">
         <v>19.232800000000001</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L228">
+        <v>18.113600000000002</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -24978,8 +25668,11 @@
       <c r="K229">
         <v>9.9222699999999993</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L229">
+        <v>9.3394200000000005</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -25013,8 +25706,11 @@
       <c r="K230">
         <v>41.348100000000002</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L230">
+        <v>39.2239</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -25048,8 +25744,11 @@
       <c r="K231">
         <v>41.652500000000003</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L231">
+        <v>39.485900000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -25083,8 +25782,11 @@
       <c r="K232">
         <v>19.381499999999999</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L232">
+        <v>18.227499999999999</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -25118,8 +25820,11 @@
       <c r="K233">
         <v>5.3562599999999998</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L233">
+        <v>5.0555700000000003</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -25153,8 +25858,11 @@
       <c r="K234">
         <v>1.7102900000000001</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L234">
+        <v>1.69112</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -25188,8 +25896,11 @@
       <c r="K235">
         <v>1.54234</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L235">
+        <v>1.51637</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -25223,8 +25934,11 @@
       <c r="K236">
         <v>4.2169699999999999</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L236">
+        <v>4.0604500000000003</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -25258,8 +25972,11 @@
       <c r="K237">
         <v>18.486000000000001</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L237">
+        <v>17.210999999999999</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -25293,8 +26010,11 @@
       <c r="K238">
         <v>2.6731699999999998</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L238">
+        <v>2.5416699999999999</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -25328,8 +26048,11 @@
       <c r="K239">
         <v>3.0393599999999998</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L239">
+        <v>2.9818699999999998</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -25363,8 +26086,11 @@
       <c r="K240">
         <v>2.84693</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L240">
+        <v>2.7887300000000002</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -25398,8 +26124,11 @@
       <c r="K241">
         <v>1.7384900000000001</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L241">
+        <v>1.70244</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -25433,8 +26162,11 @@
       <c r="K242">
         <v>1.62496</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L242">
+        <v>1.60355</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -25468,8 +26200,11 @@
       <c r="K243">
         <v>3.3694899999999999</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L243">
+        <v>3.3519100000000002</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -25503,8 +26238,11 @@
       <c r="K244">
         <v>3.9540199999999999</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L244">
+        <v>3.8437999999999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -25538,8 +26276,11 @@
       <c r="K245">
         <v>4.1319400000000002</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L245">
+        <v>4.0588899999999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -25573,8 +26314,11 @@
       <c r="K246">
         <v>3.1819700000000002</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L246">
+        <v>3.1902499999999998</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -25608,8 +26352,11 @@
       <c r="K247">
         <v>2.95052</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L247">
+        <v>2.9484400000000002</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -25643,8 +26390,11 @@
       <c r="K248">
         <v>18.311900000000001</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L248">
+        <v>17.216000000000001</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -25678,8 +26428,11 @@
       <c r="K249">
         <v>4.3520000000000003</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L249">
+        <v>4.1710599999999998</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -25713,8 +26466,11 @@
       <c r="K250">
         <v>1.7442599999999999</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L250">
+        <v>1.7353400000000001</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -25748,8 +26504,11 @@
       <c r="K251">
         <v>6.3515800000000002</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L251">
+        <v>6.01546</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -25783,8 +26542,11 @@
       <c r="K252">
         <v>1.7162999999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L252">
+        <v>1.68086</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -25818,8 +26580,11 @@
       <c r="K253">
         <v>2.6359900000000001</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L253">
+        <v>2.5482399999999998</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -25853,8 +26618,11 @@
       <c r="K254">
         <v>30.470199999999998</v>
       </c>
-    </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L254">
+        <v>27.367699999999999</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -25888,8 +26656,11 @@
       <c r="K255">
         <v>3.1374599999999999</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L255">
+        <v>3.0417999999999998</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -25923,8 +26694,11 @@
       <c r="K256">
         <v>2.3191099999999998</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L256">
+        <v>2.2839999999999998</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -25958,8 +26732,11 @@
       <c r="K257">
         <v>2.3997099999999998</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L257">
+        <v>2.3414799999999998</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -25993,8 +26770,11 @@
       <c r="K258">
         <v>5.5408200000000001</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L258">
+        <v>5.2843200000000001</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -26028,8 +26808,11 @@
       <c r="K259">
         <v>36.311999999999998</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L259">
+        <v>34.027900000000002</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -26063,8 +26846,11 @@
       <c r="K260">
         <v>4.2112499999999997</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L260">
+        <v>3.9891999999999999</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -26098,8 +26884,11 @@
       <c r="K261">
         <v>2.42652</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L261">
+        <v>2.3677899999999998</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -26133,8 +26922,11 @@
       <c r="K262">
         <v>2.2371400000000001</v>
       </c>
-    </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L262">
+        <v>2.1875300000000002</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -26168,8 +26960,11 @@
       <c r="K263">
         <v>1.6211899999999999</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L263">
+        <v>1.59413</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -26203,8 +26998,11 @@
       <c r="K264">
         <v>3.97627</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L264">
+        <v>3.8048000000000002</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -26238,8 +27036,11 @@
       <c r="K265">
         <v>3.0190600000000001</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L265">
+        <v>2.8298399999999999</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -26273,8 +27074,11 @@
       <c r="K266">
         <v>2.5758999999999999</v>
       </c>
-    </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L266">
+        <v>2.50379</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -26308,8 +27112,11 @@
       <c r="K267">
         <v>1.80874</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L267">
+        <v>1.78525</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -26343,8 +27150,11 @@
       <c r="K268">
         <v>2.87738</v>
       </c>
-    </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L268">
+        <v>2.78321</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -26378,8 +27188,11 @@
       <c r="K269">
         <v>4.6992799999999999</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L269">
+        <v>4.5118200000000002</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -26413,8 +27226,11 @@
       <c r="K270">
         <v>18.4329</v>
       </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L270">
+        <v>17.334399999999999</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -26448,8 +27264,11 @@
       <c r="K271">
         <v>5.4314600000000004</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L271">
+        <v>5.2878600000000002</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -26483,8 +27302,11 @@
       <c r="K272">
         <v>2.6108799999999999</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L272">
+        <v>2.5507499999999999</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -26518,8 +27340,11 @@
       <c r="K273">
         <v>2.51674</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L273">
+        <v>2.45262</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -26553,8 +27378,11 @@
       <c r="K274">
         <v>2.19171</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L274">
+        <v>2.1431</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -26588,8 +27416,11 @@
       <c r="K275">
         <v>2.9729999999999999</v>
       </c>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L275">
+        <v>2.9616099999999999</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -26623,8 +27454,11 @@
       <c r="K276">
         <v>3.8396599999999999</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L276">
+        <v>3.7606799999999998</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -26658,8 +27492,11 @@
       <c r="K277">
         <v>2.82748</v>
       </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L277">
+        <v>2.71766</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -26693,8 +27530,11 @@
       <c r="K278">
         <v>2.6181299999999998</v>
       </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L278">
+        <v>2.56427</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -26728,8 +27568,11 @@
       <c r="K279">
         <v>3.3694000000000002</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L279">
+        <v>3.2507999999999999</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -26763,8 +27606,11 @@
       <c r="K280">
         <v>2.4351500000000001</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L280">
+        <v>2.3616799999999998</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -26798,8 +27644,11 @@
       <c r="K281">
         <v>18.348199999999999</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L281">
+        <v>17.246099999999998</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -26833,8 +27682,11 @@
       <c r="K282">
         <v>2.64161</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L282">
+        <v>2.5647199999999999</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -26868,8 +27720,11 @@
       <c r="K283">
         <v>3.1341600000000001</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L283">
+        <v>3.10873</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -26903,8 +27758,11 @@
       <c r="K284">
         <v>2.1963200000000001</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L284">
+        <v>2.1371000000000002</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -26938,8 +27796,11 @@
       <c r="K285">
         <v>2.1540699999999999</v>
       </c>
-    </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L285">
+        <v>2.0860500000000002</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -26973,8 +27834,11 @@
       <c r="K286">
         <v>3.2767599999999999</v>
       </c>
-    </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L286">
+        <v>3.2239499999999999</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -27008,8 +27872,11 @@
       <c r="K287">
         <v>1.9952000000000001</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L287">
+        <v>1.9704699999999999</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -27043,8 +27910,11 @@
       <c r="K288">
         <v>2.9887600000000001</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L288">
+        <v>2.9801899999999999</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -27078,8 +27948,11 @@
       <c r="K289">
         <v>2.3355600000000001</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L289">
+        <v>2.2856200000000002</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -27113,8 +27986,11 @@
       <c r="K290">
         <v>4.0724999999999998</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L290">
+        <v>3.9656500000000001</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -27148,8 +28024,11 @@
       <c r="K291">
         <v>2.2160799999999998</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L291">
+        <v>2.18018</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>291</v>
       </c>
@@ -27179,6 +28058,9 @@
       </c>
       <c r="K292" t="s">
         <v>300</v>
+      </c>
+      <c r="L292" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avoid storing when simplification is invalid
</commit_message>
<xml_diff>
--- a/app/result.xlsx
+++ b/app/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QOC\MeshSimplification-Mobile\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C50EA-972B-4C38-BD31-E4734E7DB1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA0097-A5DA-45D4-9C47-929ACC49E5A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
   <si>
     <t>mesh0</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>Optimize buildEdge data structure</t>
+  </si>
+  <si>
+    <t>Avoid Store when invalid</t>
   </si>
 </sst>
 </file>
@@ -29497,10 +29500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N292"/>
+  <dimension ref="A1:O292"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N291"/>
+    <sheetView tabSelected="1" topLeftCell="J273" workbookViewId="0">
+      <selection activeCell="O293" sqref="O293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29518,9 +29521,10 @@
     <col min="12" max="12" width="28.85546875" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" customWidth="1"/>
     <col min="14" max="14" width="32.28515625" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -29563,8 +29567,11 @@
       <c r="N1">
         <v>15.4398</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1">
+        <v>15.5718</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -29607,8 +29614,11 @@
       <c r="N2">
         <v>14.2712</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>14.289300000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -29651,8 +29661,11 @@
       <c r="N3">
         <v>13.6333</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>13.775600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -29695,8 +29708,11 @@
       <c r="N4">
         <v>0.53498400000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0.53251599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -29739,8 +29755,11 @@
       <c r="N5">
         <v>0.79560399999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0.78981800000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -29783,8 +29802,11 @@
       <c r="N6">
         <v>0.45347799999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>0.44909399999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -29827,8 +29849,11 @@
       <c r="N7">
         <v>4.5268000000000003E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>4.6575999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -29871,8 +29896,11 @@
       <c r="N8">
         <v>0.31730999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0.31963999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -29915,8 +29943,11 @@
       <c r="N9">
         <v>1.34212</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>1.3433299999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -29959,8 +29990,11 @@
       <c r="N10">
         <v>0.285078</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>0.28066000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -30003,8 +30037,11 @@
       <c r="N11">
         <v>0.401756</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0.39807399999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -30047,8 +30084,11 @@
       <c r="N12">
         <v>7.6546100000000006E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>7.2031899999999996E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -30091,8 +30131,11 @@
       <c r="N13">
         <v>2.5206</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>2.4946899999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -30135,8 +30178,11 @@
       <c r="N14">
         <v>24.055</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>24.2685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -30179,8 +30225,11 @@
       <c r="N15">
         <v>0.242344</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0.238348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -30223,8 +30272,11 @@
       <c r="N16">
         <v>0.37320199999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0.371778</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -30267,8 +30319,11 @@
       <c r="N17">
         <v>0.34009</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>0.33909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -30311,8 +30366,11 @@
       <c r="N18">
         <v>0.30277399999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>0.29827799999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -30355,8 +30413,11 @@
       <c r="N19">
         <v>0.47844399999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>0.479159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -30399,8 +30460,11 @@
       <c r="N20">
         <v>1.49959</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1.4821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -30443,8 +30507,11 @@
       <c r="N21">
         <v>6.1955999999999997E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>6.0201999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -30487,8 +30554,11 @@
       <c r="N22">
         <v>3.0853999999999999E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>3.0764E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -30531,8 +30601,11 @@
       <c r="N23">
         <v>0.77614099999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>0.77199700000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -30575,8 +30648,11 @@
       <c r="N24">
         <v>1.1556200000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1.1542600000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -30619,8 +30695,11 @@
       <c r="N25">
         <v>27.4834</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>27.743600000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -30663,8 +30742,11 @@
       <c r="N26">
         <v>0.350134</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>0.34861199999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -30707,8 +30789,11 @@
       <c r="N27">
         <v>0.77408200000000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>0.77349699999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -30751,8 +30836,11 @@
       <c r="N28">
         <v>8.85962E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>8.9976200000000006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -30795,8 +30883,11 @@
       <c r="N29">
         <v>0.44570199999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>0.4501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -30839,8 +30930,11 @@
       <c r="N30">
         <v>0.53459000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>0.53727199999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -30883,8 +30977,11 @@
       <c r="N31">
         <v>0.26716699999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>0.267708</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -30927,8 +31024,11 @@
       <c r="N32">
         <v>0.94357599999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>0.94439200000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -30971,8 +31071,11 @@
       <c r="N33">
         <v>0.37707600000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>0.37641200000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -31015,8 +31118,11 @@
       <c r="N34">
         <v>0.203287</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>0.20701600000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -31059,8 +31165,11 @@
       <c r="N35">
         <v>1.43655</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>1.4430400000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -31103,8 +31212,11 @@
       <c r="N36">
         <v>13.665900000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>13.7668</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -31147,8 +31259,11 @@
       <c r="N37">
         <v>1.11643</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>1.1157699999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -31191,8 +31306,11 @@
       <c r="N38">
         <v>1.04915</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1.04956</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -31235,8 +31353,11 @@
       <c r="N39">
         <v>0.14677799999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>0.14945600000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -31279,8 +31400,11 @@
       <c r="N40">
         <v>1.08186</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>1.0871299999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -31323,8 +31447,11 @@
       <c r="N41">
         <v>0.48868200000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>0.48546400000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -31367,8 +31494,11 @@
       <c r="N42">
         <v>0.69207300000000005</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>0.69368700000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -31411,8 +31541,11 @@
       <c r="N43">
         <v>0.59553599999999995</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>0.59923800000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -31455,8 +31588,11 @@
       <c r="N44">
         <v>0.61663999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>0.61909599999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -31499,8 +31635,11 @@
       <c r="N45">
         <v>0.11766</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>0.11777600000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -31543,8 +31682,11 @@
       <c r="N46">
         <v>0.73192000000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>0.735232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -31587,8 +31729,11 @@
       <c r="N47">
         <v>15.4833</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>15.6175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -31631,8 +31776,11 @@
       <c r="N48">
         <v>0.17369399999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>0.17546400000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -31675,8 +31823,11 @@
       <c r="N49">
         <v>0.88602700000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>0.89066800000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -31719,8 +31870,11 @@
       <c r="N50">
         <v>0.20765700000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>0.20811499999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -31763,8 +31917,11 @@
       <c r="N51">
         <v>0.26594899999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>0.266517</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -31807,8 +31964,11 @@
       <c r="N52">
         <v>1.5911999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>1.61456</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -31851,8 +32011,11 @@
       <c r="N53">
         <v>0.90637800000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>0.91453600000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -31895,8 +32058,11 @@
       <c r="N54">
         <v>0.16189200000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>0.158662</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -31939,8 +32105,11 @@
       <c r="N55">
         <v>0.71643800000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>0.71836299999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -31983,8 +32152,11 @@
       <c r="N56">
         <v>0.98343499999999995</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>0.97289199999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -32027,8 +32199,11 @@
       <c r="N57">
         <v>0.56564000000000003</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>0.561222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -32071,8 +32246,11 @@
       <c r="N58">
         <v>13.5465</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>13.637499999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -32115,8 +32293,11 @@
       <c r="N59">
         <v>0.132606</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>0.134488</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -32159,8 +32340,11 @@
       <c r="N60">
         <v>0.215892</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>0.21736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -32203,8 +32387,11 @@
       <c r="N61">
         <v>0.19169800000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>0.18912499999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -32247,8 +32434,11 @@
       <c r="N62">
         <v>1.7056800000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>1.6971700000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -32291,8 +32481,11 @@
       <c r="N63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -32335,8 +32528,11 @@
       <c r="N64">
         <v>1.0432399999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>1.0523100000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -32379,8 +32575,11 @@
       <c r="N65">
         <v>2.6859700000000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <v>2.7039599999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -32423,8 +32622,11 @@
       <c r="N66">
         <v>6.2319100000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <v>6.2651599999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -32467,8 +32669,11 @@
       <c r="N67">
         <v>0.46028999999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <v>0.46511000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -32511,8 +32716,11 @@
       <c r="N68">
         <v>0.47641600000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68">
+        <v>0.47834199999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -32555,8 +32763,11 @@
       <c r="N69">
         <v>15.4335</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69">
+        <v>15.5776</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -32599,8 +32810,11 @@
       <c r="N70">
         <v>0.34015200000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70">
+        <v>0.34203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -32643,8 +32857,11 @@
       <c r="N71">
         <v>8.1379999999999994E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71">
+        <v>7.7473799999999995E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -32687,8 +32904,11 @@
       <c r="N72">
         <v>0.22048200000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72">
+        <v>0.21732499999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -32731,8 +32951,11 @@
       <c r="N73">
         <v>0.19276199999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73">
+        <v>0.18890399999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -32775,8 +32998,11 @@
       <c r="N74">
         <v>0.107714</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74">
+        <v>0.106978</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -32819,8 +33045,11 @@
       <c r="N75">
         <v>0.30678</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75">
+        <v>0.30958400000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -32863,8 +33092,11 @@
       <c r="N76">
         <v>0.11107599999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76">
+        <v>0.111066</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -32907,8 +33139,11 @@
       <c r="N77">
         <v>1.07731</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77">
+        <v>1.08277</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -32951,8 +33186,11 @@
       <c r="N78">
         <v>0.34548200000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78">
+        <v>0.35063800000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -32995,8 +33233,11 @@
       <c r="N79">
         <v>0.233178</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79">
+        <v>0.23528199999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -33039,8 +33280,11 @@
       <c r="N80">
         <v>13.4986</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80">
+        <v>13.6317</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -33083,8 +33327,11 @@
       <c r="N81">
         <v>0.17819199999999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81">
+        <v>0.179174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -33127,8 +33374,11 @@
       <c r="N82">
         <v>0.33156999999999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82">
+        <v>0.32923999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -33171,8 +33421,11 @@
       <c r="N83">
         <v>0.80304600000000004</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83">
+        <v>0.80803599999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -33215,8 +33468,11 @@
       <c r="N84">
         <v>2.7194799999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84">
+        <v>2.7249599999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -33259,8 +33515,11 @@
       <c r="N85">
         <v>1.1167199999999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85">
+        <v>1.1208499999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -33303,8 +33562,11 @@
       <c r="N86">
         <v>1.00414</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86">
+        <v>0.99102900000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -33347,8 +33609,11 @@
       <c r="N87">
         <v>5.8077900000000002E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87">
+        <v>5.74799E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -33391,8 +33656,11 @@
       <c r="N88">
         <v>5.2443999999999998E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88">
+        <v>5.1903999999999999E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -33435,8 +33703,11 @@
       <c r="N89">
         <v>0.134212</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89">
+        <v>0.13561599999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -33479,8 +33750,11 @@
       <c r="N90">
         <v>5.5590199999999999E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90">
+        <v>5.5176200000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -33523,8 +33797,11 @@
       <c r="N91">
         <v>15.376099999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91">
+        <v>15.527200000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -33567,8 +33844,11 @@
       <c r="N92">
         <v>0.28340900000000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92">
+        <v>0.290184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -33611,8 +33891,11 @@
       <c r="N93">
         <v>0.23896200000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93">
+        <v>0.23418700000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -33655,8 +33938,11 @@
       <c r="N94">
         <v>0.16789299999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94">
+        <v>0.16434599999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -33699,8 +33985,11 @@
       <c r="N95">
         <v>0.56601400000000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95">
+        <v>0.55445</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -33743,8 +34032,11 @@
       <c r="N96" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -33787,8 +34079,11 @@
       <c r="N97">
         <v>0.105418</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97">
+        <v>0.10248400000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -33831,8 +34126,11 @@
       <c r="N98">
         <v>0.17005600000000001</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98">
+        <v>0.16943</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -33875,8 +34173,11 @@
       <c r="N99">
         <v>0.135798</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99">
+        <v>0.13259000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -33919,8 +34220,11 @@
       <c r="N100">
         <v>2.0916299999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100">
+        <v>2.1073400000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -33963,8 +34267,11 @@
       <c r="N101">
         <v>0.24310399999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101">
+        <v>0.244004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -34007,8 +34314,11 @@
       <c r="N102">
         <v>13.7073</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102">
+        <v>13.834</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -34051,8 +34361,11 @@
       <c r="N103">
         <v>1.85389</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103">
+        <v>1.8689800000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -34095,8 +34408,11 @@
       <c r="N104">
         <v>0.58099500000000004</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104">
+        <v>0.57970699999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -34139,8 +34455,11 @@
       <c r="N105">
         <v>0.54578400000000005</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105">
+        <v>0.54503199999999996</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -34183,8 +34502,11 @@
       <c r="N106">
         <v>0.130632</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106">
+        <v>0.131354</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -34227,8 +34549,11 @@
       <c r="N107">
         <v>0.53447199999999995</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107">
+        <v>0.52868199999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -34271,8 +34596,11 @@
       <c r="N108">
         <v>5.4570199999999999E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108">
+        <v>5.4944199999999999E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -34315,8 +34643,11 @@
       <c r="N109">
         <v>6.1626E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109">
+        <v>5.7702000000000003E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -34359,8 +34690,11 @@
       <c r="N110">
         <v>0.26800800000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110">
+        <v>0.261957</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -34403,8 +34737,11 @@
       <c r="N111">
         <v>0.11409</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O111">
+        <v>0.110744</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -34447,8 +34784,11 @@
       <c r="N112">
         <v>5.0649800000000002E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112">
+        <v>5.0781800000000002E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -34491,8 +34831,11 @@
       <c r="N113">
         <v>13.574400000000001</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113">
+        <v>13.6944</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -34535,8 +34878,11 @@
       <c r="N114">
         <v>13.777799999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114">
+        <v>13.884399999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -34579,8 +34925,11 @@
       <c r="N115">
         <v>0.107332</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115">
+        <v>0.108464</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -34623,8 +34972,11 @@
       <c r="N116">
         <v>0.73741599999999996</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116">
+        <v>0.73848400000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -34667,8 +35019,11 @@
       <c r="N117">
         <v>0.107408</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117">
+        <v>0.10574799999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -34711,8 +35066,11 @@
       <c r="N118">
         <v>0.51155099999999998</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118">
+        <v>0.50424999999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -34755,8 +35113,11 @@
       <c r="N119">
         <v>0.20968100000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119">
+        <v>0.209284</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -34799,8 +35160,11 @@
       <c r="N120">
         <v>0.181252</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120">
+        <v>0.17826400000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -34843,8 +35207,11 @@
       <c r="N121">
         <v>1.3821300000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121">
+        <v>1.3856599999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -34887,8 +35254,11 @@
       <c r="N122">
         <v>2.2656100000000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122">
+        <v>2.30036</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -34931,8 +35301,11 @@
       <c r="N123">
         <v>7.3017700000000003</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123">
+        <v>7.2673800000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -34975,8 +35348,11 @@
       <c r="N124">
         <v>1.19299</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124">
+        <v>1.2098800000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -35019,8 +35395,11 @@
       <c r="N125">
         <v>15.5739</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125">
+        <v>15.731299999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -35063,8 +35442,11 @@
       <c r="N126">
         <v>3.4939300000000002</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O126">
+        <v>3.48102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -35107,8 +35489,11 @@
       <c r="N127">
         <v>9.3607999999999997E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O127">
+        <v>9.1044100000000003E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -35151,8 +35536,11 @@
       <c r="N128">
         <v>1.4521900000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O128">
+        <v>1.4577500000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -35195,8 +35583,11 @@
       <c r="N129">
         <v>1.37507</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O129">
+        <v>1.3904000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -35239,8 +35630,11 @@
       <c r="N130">
         <v>0.21403700000000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O130">
+        <v>0.21692900000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -35283,8 +35677,11 @@
       <c r="N131">
         <v>6.6673099999999996</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O131">
+        <v>6.6919399999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -35327,8 +35724,11 @@
       <c r="N132">
         <v>0.55538399999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O132">
+        <v>0.56934399999999996</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -35371,8 +35771,11 @@
       <c r="N133">
         <v>1.67597</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O133">
+        <v>1.6949000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -35415,8 +35818,11 @@
       <c r="N134">
         <v>2.2272699999999999</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O134">
+        <v>2.2261099999999998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -35459,8 +35865,11 @@
       <c r="N135">
         <v>3.1464300000000001</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O135">
+        <v>3.1496200000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -35503,8 +35912,11 @@
       <c r="N136">
         <v>7.7956099999999999</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O136">
+        <v>7.8534600000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -35547,8 +35959,11 @@
       <c r="N137">
         <v>5.4433400000000001</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O137">
+        <v>5.4809599999999996</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -35591,8 +36006,11 @@
       <c r="N138">
         <v>2.5473699999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O138">
+        <v>2.5630999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -35635,8 +36053,11 @@
       <c r="N139">
         <v>19.287199999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O139">
+        <v>19.432200000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -35679,8 +36100,11 @@
       <c r="N140">
         <v>18.508500000000002</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O140">
+        <v>18.566600000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -35723,8 +36147,11 @@
       <c r="N141">
         <v>1.36283</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O141">
+        <v>1.3770800000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -35767,8 +36194,11 @@
       <c r="N142">
         <v>2.9706999999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O142">
+        <v>2.99064</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -35811,8 +36241,11 @@
       <c r="N143">
         <v>2.6986400000000001</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O143">
+        <v>2.69001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -35855,8 +36288,11 @@
       <c r="N144">
         <v>0.32741999999999999</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O144">
+        <v>0.32470199999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -35899,8 +36335,11 @@
       <c r="N145">
         <v>1.93492</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O145">
+        <v>1.9606300000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -35943,8 +36382,11 @@
       <c r="N146">
         <v>0.64917499999999995</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O146">
+        <v>0.65442100000000003</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -35987,8 +36429,11 @@
       <c r="N147">
         <v>15.4414</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O147">
+        <v>15.5815</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -36031,8 +36476,11 @@
       <c r="N148">
         <v>4.2475899999999998</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O148">
+        <v>4.25366</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -36075,8 +36523,11 @@
       <c r="N149">
         <v>3.5513400000000002</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O149">
+        <v>3.5617299999999998</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -36119,8 +36570,11 @@
       <c r="N150">
         <v>6.3324199999999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O150">
+        <v>6.3349799999999998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -36163,8 +36617,11 @@
       <c r="N151">
         <v>9.9021699999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O151">
+        <v>9.9680700000000009</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -36207,8 +36664,11 @@
       <c r="N152">
         <v>0.495226</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O152">
+        <v>0.50619800000000004</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -36251,8 +36711,11 @@
       <c r="N153">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O153">
+        <v>1.4712499999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -36295,8 +36758,11 @@
       <c r="N154">
         <v>2.1316799999999998</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O154">
+        <v>2.1365500000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -36339,8 +36805,11 @@
       <c r="N155">
         <v>2.9822899999999999</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O155">
+        <v>2.99932</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -36383,8 +36852,11 @@
       <c r="N156">
         <v>4.1834699999999998</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O156">
+        <v>4.2275499999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -36427,8 +36899,11 @@
       <c r="N157">
         <v>11.237500000000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O157">
+        <v>11.338900000000001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -36471,8 +36946,11 @@
       <c r="N158">
         <v>15.4819</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O158">
+        <v>15.619</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -36515,8 +36993,11 @@
       <c r="N159">
         <v>2.4914999999999998</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O159">
+        <v>2.5288499999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -36559,8 +37040,11 @@
       <c r="N160">
         <v>0.77954000000000001</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O160">
+        <v>0.78138399999999997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -36603,8 +37087,11 @@
       <c r="N161">
         <v>1.46519</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O161">
+        <v>1.4528099999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -36647,8 +37134,11 @@
       <c r="N162">
         <v>4.4945899999999996</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O162">
+        <v>4.5239000000000003</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -36691,8 +37181,11 @@
       <c r="N163">
         <v>3.61836</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O163">
+        <v>3.67082</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -36735,8 +37228,11 @@
       <c r="N164">
         <v>0.51579799999999998</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O164">
+        <v>0.51858199999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -36779,8 +37275,11 @@
       <c r="N165">
         <v>2.2900299999999998</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O165">
+        <v>2.2839100000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -36823,8 +37322,11 @@
       <c r="N166">
         <v>2.5358800000000001</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O166">
+        <v>2.5479699999999998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -36867,8 +37369,11 @@
       <c r="N167">
         <v>3.0310299999999999</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O167">
+        <v>3.02556</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -36911,8 +37416,11 @@
       <c r="N168">
         <v>2.22499</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O168">
+        <v>2.2591800000000002</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -36955,8 +37463,11 @@
       <c r="N169">
         <v>24.210100000000001</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O169">
+        <v>24.4178</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -36999,8 +37510,11 @@
       <c r="N170">
         <v>3.7332299999999998</v>
       </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O170">
+        <v>3.7647400000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -37043,8 +37557,11 @@
       <c r="N171">
         <v>0.59284400000000004</v>
       </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O171">
+        <v>0.60429200000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -37087,8 +37604,11 @@
       <c r="N172">
         <v>0.50270000000000004</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O172">
+        <v>0.51489200000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -37131,8 +37651,11 @@
       <c r="N173">
         <v>0.81100799999999995</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O173">
+        <v>0.81729399999999996</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -37175,8 +37698,11 @@
       <c r="N174">
         <v>1.0552900000000001</v>
       </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O174">
+        <v>1.0565199999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -37219,8 +37745,11 @@
       <c r="N175">
         <v>0.487516</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O175">
+        <v>0.48621799999999998</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -37263,8 +37792,11 @@
       <c r="N176">
         <v>2.2563900000000001</v>
       </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O176">
+        <v>2.2756799999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -37307,8 +37839,11 @@
       <c r="N177">
         <v>2.0083500000000001</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O177">
+        <v>2.00156</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -37351,8 +37886,11 @@
       <c r="N178">
         <v>1.53376</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O178">
+        <v>1.5299100000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -37395,8 +37933,11 @@
       <c r="N179">
         <v>2.78721</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O179">
+        <v>2.8279100000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -37439,8 +37980,11 @@
       <c r="N180">
         <v>15.6662</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O180">
+        <v>15.8886</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -37483,8 +38027,11 @@
       <c r="N181">
         <v>1.09789</v>
       </c>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O181">
+        <v>1.0918699999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -37527,8 +38074,11 @@
       <c r="N182">
         <v>4.4585100000000004</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O182">
+        <v>4.49444</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -37571,8 +38121,11 @@
       <c r="N183">
         <v>0.89832400000000001</v>
       </c>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O183">
+        <v>0.89994399999999997</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -37615,8 +38168,11 @@
       <c r="N184">
         <v>0.26524399999999998</v>
       </c>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O184">
+        <v>0.26260099999999997</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -37659,8 +38215,11 @@
       <c r="N185">
         <v>0.66358799999999996</v>
       </c>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O185">
+        <v>0.67093199999999997</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -37703,8 +38262,11 @@
       <c r="N186">
         <v>2.15137</v>
       </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O186">
+        <v>2.1594000000000002</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -37747,8 +38309,11 @@
       <c r="N187">
         <v>0.310004</v>
       </c>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O187">
+        <v>0.31454799999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -37791,8 +38356,11 @@
       <c r="N188">
         <v>2.9549799999999999</v>
       </c>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O188">
+        <v>2.98305</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -37835,8 +38403,11 @@
       <c r="N189">
         <v>5.3386000000000003E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O189">
+        <v>5.2528100000000001E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -37879,8 +38450,11 @@
       <c r="N190">
         <v>0.28720000000000001</v>
       </c>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O190">
+        <v>0.28782999999999997</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -37923,8 +38497,11 @@
       <c r="N191">
         <v>15.544</v>
       </c>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O191">
+        <v>15.724600000000001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -37967,8 +38544,11 @@
       <c r="N192">
         <v>3.11599</v>
       </c>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O192">
+        <v>3.1482999999999999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -38011,8 +38591,11 @@
       <c r="N193">
         <v>1.0710500000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O193">
+        <v>1.0888199999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -38055,8 +38638,11 @@
       <c r="N194">
         <v>0.54073599999999999</v>
       </c>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O194">
+        <v>0.53598599999999996</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -38099,8 +38685,11 @@
       <c r="N195">
         <v>0.54820000000000002</v>
       </c>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O195">
+        <v>0.54852800000000002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -38143,8 +38732,11 @@
       <c r="N196">
         <v>1.4617</v>
       </c>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O196">
+        <v>1.4539500000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -38187,8 +38779,11 @@
       <c r="N197">
         <v>1.0346599999999999</v>
       </c>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O197">
+        <v>1.0381899999999999</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -38231,8 +38826,11 @@
       <c r="N198">
         <v>0.38901799999999997</v>
       </c>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O198">
+        <v>0.38761800000000002</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -38275,8 +38873,11 @@
       <c r="N199">
         <v>3.7327900000000001</v>
       </c>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O199">
+        <v>3.7329400000000001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -38319,8 +38920,11 @@
       <c r="N200">
         <v>0.98132399999999997</v>
       </c>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O200">
+        <v>0.98834999999999995</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -38363,8 +38967,11 @@
       <c r="N201">
         <v>0.74457399999999996</v>
       </c>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O201">
+        <v>0.75776600000000005</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -38407,8 +39014,11 @@
       <c r="N202">
         <v>13.847300000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O202">
+        <v>13.987</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -38451,8 +39061,11 @@
       <c r="N203">
         <v>0.36372599999999999</v>
       </c>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O203">
+        <v>0.36553400000000003</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -38495,8 +39108,11 @@
       <c r="N204">
         <v>1.30853</v>
       </c>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O204">
+        <v>1.3205100000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -38539,8 +39155,11 @@
       <c r="N205">
         <v>0.22275300000000001</v>
       </c>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O205">
+        <v>0.21998000000000001</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -38583,8 +39202,11 @@
       <c r="N206">
         <v>1.4560999999999999</v>
       </c>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O206">
+        <v>1.45943</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -38627,8 +39249,11 @@
       <c r="N207">
         <v>0.35073199999999999</v>
       </c>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O207">
+        <v>0.348806</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -38671,8 +39296,11 @@
       <c r="N208">
         <v>0.33435199999999998</v>
       </c>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O208">
+        <v>0.33061800000000002</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -38715,8 +39343,11 @@
       <c r="N209">
         <v>1.1307499999999999</v>
       </c>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O209">
+        <v>1.1460999999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -38759,8 +39390,11 @@
       <c r="N210">
         <v>9.9461900000000006E-2</v>
       </c>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O210">
+        <v>0.10091600000000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -38803,8 +39437,11 @@
       <c r="N211">
         <v>3.47071</v>
       </c>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O211">
+        <v>3.4727399999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -38847,8 +39484,11 @@
       <c r="N212">
         <v>8.7629799999999994E-2</v>
       </c>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O212">
+        <v>8.8483800000000001E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -38891,8 +39531,11 @@
       <c r="N213">
         <v>14.013400000000001</v>
       </c>
-    </row>
-    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O213">
+        <v>14.1181</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -38935,8 +39578,11 @@
       <c r="N214">
         <v>383.65499999999997</v>
       </c>
-    </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O214">
+        <v>388.68599999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -38979,8 +39625,11 @@
       <c r="N215">
         <v>15.315899999999999</v>
       </c>
-    </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O215">
+        <v>15.478</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -39023,8 +39672,11 @@
       <c r="N216">
         <v>14.122400000000001</v>
       </c>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O216">
+        <v>14.207800000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -39067,8 +39719,11 @@
       <c r="N217">
         <v>14.139799999999999</v>
       </c>
-    </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O217">
+        <v>14.2821</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -39111,8 +39766,11 @@
       <c r="N218">
         <v>27.884699999999999</v>
       </c>
-    </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O218">
+        <v>28.094899999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -39155,8 +39813,11 @@
       <c r="N219">
         <v>6.5077199999999999</v>
       </c>
-    </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O219">
+        <v>6.5498399999999997</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -39199,8 +39860,11 @@
       <c r="N220">
         <v>13.615600000000001</v>
       </c>
-    </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O220">
+        <v>13.7476</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -39243,8 +39907,11 @@
       <c r="N221">
         <v>12.257400000000001</v>
       </c>
-    </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O221">
+        <v>12.385400000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -39287,8 +39954,11 @@
       <c r="N222">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O222">
+        <v>12.3264</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -39331,8 +40001,11 @@
       <c r="N223">
         <v>15.571300000000001</v>
       </c>
-    </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O223">
+        <v>15.7356</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -39375,8 +40048,11 @@
       <c r="N224">
         <v>13.7196</v>
       </c>
-    </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O224">
+        <v>13.815899999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -39419,8 +40095,11 @@
       <c r="N225">
         <v>22.584</v>
       </c>
-    </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O225">
+        <v>22.739599999999999</v>
+      </c>
+    </row>
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -39463,8 +40142,11 @@
       <c r="N226">
         <v>13.6645</v>
       </c>
-    </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O226">
+        <v>13.8286</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -39507,8 +40189,11 @@
       <c r="N227">
         <v>13.694900000000001</v>
       </c>
-    </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O227">
+        <v>13.8047</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -39551,8 +40236,11 @@
       <c r="N228">
         <v>14.1084</v>
       </c>
-    </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O228">
+        <v>14.2234</v>
+      </c>
+    </row>
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -39595,8 +40283,11 @@
       <c r="N229">
         <v>6.4279999999999999</v>
       </c>
-    </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O229">
+        <v>6.4939299999999998</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -39639,8 +40330,11 @@
       <c r="N230">
         <v>33.764099999999999</v>
       </c>
-    </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O230">
+        <v>33.987900000000003</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -39683,8 +40377,11 @@
       <c r="N231">
         <v>33.826300000000003</v>
       </c>
-    </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O231">
+        <v>34.060299999999998</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -39727,8 +40424,11 @@
       <c r="N232">
         <v>14.162000000000001</v>
       </c>
-    </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O232">
+        <v>14.260300000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -39771,8 +40471,11 @@
       <c r="N233">
         <v>2.79054</v>
       </c>
-    </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O233">
+        <v>2.85467</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -39815,8 +40518,11 @@
       <c r="N234">
         <v>0.114178</v>
       </c>
-    </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O234">
+        <v>0.11863600000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -39859,8 +40565,11 @@
       <c r="N235">
         <v>4.7688099999999997E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O235">
+        <v>4.6517999999999997E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -39903,8 +40612,11 @@
       <c r="N236">
         <v>2.3112300000000001</v>
       </c>
-    </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O236">
+        <v>2.3269099999999998</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -39947,8 +40659,11 @@
       <c r="N237">
         <v>13.5632</v>
       </c>
-    </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O237">
+        <v>13.679600000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -39991,8 +40706,11 @@
       <c r="N238">
         <v>0.69702399999999998</v>
       </c>
-    </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O238">
+        <v>0.69996599999999998</v>
+      </c>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -40035,8 +40753,11 @@
       <c r="N239">
         <v>1.3035600000000001</v>
       </c>
-    </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O239">
+        <v>1.3097000000000001</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -40079,8 +40800,11 @@
       <c r="N240">
         <v>1.1269499999999999</v>
       </c>
-    </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O240">
+        <v>1.1489799999999999</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -40123,8 +40847,11 @@
       <c r="N241">
         <v>0.18735099999999999</v>
       </c>
-    </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O241">
+        <v>0.189609</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -40167,8 +40894,11 @@
       <c r="N242">
         <v>0.124128</v>
       </c>
-    </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O242">
+        <v>0.128084</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -40211,8 +40941,11 @@
       <c r="N243">
         <v>0.38757000000000003</v>
       </c>
-    </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O243">
+        <v>0.39388200000000001</v>
+      </c>
+    </row>
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -40255,8 +40988,11 @@
       <c r="N244">
         <v>1.98539</v>
       </c>
-    </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O244">
+        <v>1.9755199999999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -40299,8 +41035,11 @@
       <c r="N245">
         <v>1.9716400000000001</v>
       </c>
-    </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O245">
+        <v>1.9789600000000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -40343,8 +41082,11 @@
       <c r="N246">
         <v>0.122312</v>
       </c>
-    </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O246">
+        <v>0.11978</v>
+      </c>
+    </row>
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -40387,8 +41129,11 @@
       <c r="N247">
         <v>5.5296199999999997E-2</v>
       </c>
-    </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O247">
+        <v>5.5226200000000003E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -40431,8 +41176,11 @@
       <c r="N248">
         <v>13.541399999999999</v>
       </c>
-    </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O248">
+        <v>13.6579</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -40475,8 +41223,11 @@
       <c r="N249">
         <v>2.1157599999999999</v>
       </c>
-    </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O249">
+        <v>2.1518999999999999</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -40519,8 +41270,11 @@
       <c r="N250">
         <v>0.16520199999999999</v>
       </c>
-    </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O250">
+        <v>0.164524</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -40563,8 +41317,11 @@
       <c r="N251">
         <v>2.8762799999999999</v>
       </c>
-    </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O251">
+        <v>2.84328</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -40607,8 +41364,11 @@
       <c r="N252">
         <v>0.173347</v>
       </c>
-    </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O252">
+        <v>0.16994600000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -40651,8 +41411,11 @@
       <c r="N253">
         <v>0.92344199999999999</v>
       </c>
-    </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O253">
+        <v>0.92674400000000001</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -40695,8 +41458,11 @@
       <c r="N254">
         <v>25.971499999999999</v>
       </c>
-    </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O254">
+        <v>25.715800000000002</v>
+      </c>
+    </row>
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -40739,8 +41505,11 @@
       <c r="N255">
         <v>1.2084699999999999</v>
       </c>
-    </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O255">
+        <v>1.2203900000000001</v>
+      </c>
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -40783,8 +41552,11 @@
       <c r="N256">
         <v>0.59828800000000004</v>
       </c>
-    </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O256">
+        <v>0.59589999999999999</v>
+      </c>
+    </row>
+    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -40827,8 +41599,11 @@
       <c r="N257">
         <v>0.69210700000000003</v>
       </c>
-    </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O257">
+        <v>0.69149499999999997</v>
+      </c>
+    </row>
+    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -40871,8 +41646,11 @@
       <c r="N258">
         <v>3.2702</v>
       </c>
-    </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O258">
+        <v>3.24823</v>
+      </c>
+    </row>
+    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -40915,8 +41693,11 @@
       <c r="N259">
         <v>28.4343</v>
       </c>
-    </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O259">
+        <v>28.765899999999998</v>
+      </c>
+    </row>
+    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -40959,8 +41740,11 @@
       <c r="N260">
         <v>1.67621</v>
       </c>
-    </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O260">
+        <v>1.67157</v>
+      </c>
+    </row>
+    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -41003,8 +41787,11 @@
       <c r="N261">
         <v>0.71545199999999998</v>
       </c>
-    </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O261">
+        <v>0.71263799999999999</v>
+      </c>
+    </row>
+    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -41047,8 +41834,11 @@
       <c r="N262">
         <v>0.58153600000000005</v>
       </c>
-    </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O262">
+        <v>0.57955599999999996</v>
+      </c>
+    </row>
+    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -41091,8 +41881,11 @@
       <c r="N263">
         <v>0.101842</v>
       </c>
-    </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O263">
+        <v>0.102756</v>
+      </c>
+    </row>
+    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -41135,8 +41928,11 @@
       <c r="N264">
         <v>1.9836499999999999</v>
       </c>
-    </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O264">
+        <v>2.0087700000000002</v>
+      </c>
+    </row>
+    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -41179,8 +41975,11 @@
       <c r="N265">
         <v>1.2707900000000001</v>
       </c>
-    </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O265">
+        <v>1.28555</v>
+      </c>
+    </row>
+    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -41223,8 +42022,11 @@
       <c r="N266">
         <v>0.91881900000000005</v>
       </c>
-    </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O266">
+        <v>0.914381</v>
+      </c>
+    </row>
+    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -41267,8 +42069,11 @@
       <c r="N267">
         <v>0.25574799999999998</v>
       </c>
-    </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O267">
+        <v>0.253106</v>
+      </c>
+    </row>
+    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -41311,8 +42116,11 @@
       <c r="N268">
         <v>1.1357900000000001</v>
       </c>
-    </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O268">
+        <v>1.13585</v>
+      </c>
+    </row>
+    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -41355,8 +42163,11 @@
       <c r="N269">
         <v>2.6115400000000002</v>
       </c>
-    </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O269">
+        <v>2.6193200000000001</v>
+      </c>
+    </row>
+    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -41399,8 +42210,11 @@
       <c r="N270">
         <v>13.6675</v>
       </c>
-    </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O270">
+        <v>13.762700000000001</v>
+      </c>
+    </row>
+    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -41443,8 +42257,11 @@
       <c r="N271">
         <v>1.5402</v>
       </c>
-    </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O271">
+        <v>1.55148</v>
+      </c>
+    </row>
+    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -41487,8 +42304,11 @@
       <c r="N272">
         <v>0.92239000000000004</v>
       </c>
-    </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O272">
+        <v>0.91697600000000001</v>
+      </c>
+    </row>
+    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -41531,8 +42351,11 @@
       <c r="N273">
         <v>0.83800600000000003</v>
       </c>
-    </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O273">
+        <v>0.83366300000000004</v>
+      </c>
+    </row>
+    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -41575,8 +42398,11 @@
       <c r="N274">
         <v>0.58828499999999995</v>
       </c>
-    </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O274">
+        <v>0.59801599999999999</v>
+      </c>
+    </row>
+    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -41619,8 +42445,11 @@
       <c r="N275">
         <v>5.7671899999999998E-2</v>
       </c>
-    </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O275">
+        <v>5.9339999999999997E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -41663,8 +42492,11 @@
       <c r="N276">
         <v>0.72911899999999996</v>
       </c>
-    </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O276">
+        <v>0.72207900000000003</v>
+      </c>
+    </row>
+    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -41707,8 +42539,11 @@
       <c r="N277">
         <v>1.0476399999999999</v>
       </c>
-    </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O277">
+        <v>1.0327999999999999</v>
+      </c>
+    </row>
+    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -41751,8 +42586,11 @@
       <c r="N278">
         <v>0.93048399999999998</v>
       </c>
-    </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O278">
+        <v>0.94028400000000001</v>
+      </c>
+    </row>
+    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -41795,8 +42633,11 @@
       <c r="N279">
         <v>1.5328999999999999</v>
       </c>
-    </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O279">
+        <v>1.5239799999999999</v>
+      </c>
+    </row>
+    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -41839,8 +42680,11 @@
       <c r="N280">
         <v>0.69780200000000003</v>
       </c>
-    </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O280">
+        <v>0.69358500000000001</v>
+      </c>
+    </row>
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -41883,8 +42727,11 @@
       <c r="N281">
         <v>13.5503</v>
       </c>
-    </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O281">
+        <v>13.686999999999999</v>
+      </c>
+    </row>
+    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -41927,8 +42774,11 @@
       <c r="N282">
         <v>0.64571400000000001</v>
       </c>
-    </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O282">
+        <v>0.64471199999999995</v>
+      </c>
+    </row>
+    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -41971,8 +42821,11 @@
       <c r="N283">
         <v>0.13867399999999999</v>
       </c>
-    </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O283">
+        <v>0.13492000000000001</v>
+      </c>
+    </row>
+    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -42015,8 +42868,11 @@
       <c r="N284">
         <v>0.56059599999999998</v>
       </c>
-    </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O284">
+        <v>0.56060699999999997</v>
+      </c>
+    </row>
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -42059,8 +42915,11 @@
       <c r="N285">
         <v>0.52081599999999995</v>
       </c>
-    </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O285">
+        <v>0.52249699999999999</v>
+      </c>
+    </row>
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -42103,8 +42962,11 @@
       <c r="N286">
         <v>0.27347300000000002</v>
       </c>
-    </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O286">
+        <v>0.272623</v>
+      </c>
+    </row>
+    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -42147,8 +43009,11 @@
       <c r="N287">
         <v>0.464032</v>
       </c>
-    </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O287">
+        <v>0.460094</v>
+      </c>
+    </row>
+    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -42191,8 +43056,11 @@
       <c r="N288">
         <v>8.2464200000000001E-2</v>
       </c>
-    </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O288">
+        <v>8.0376100000000006E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -42235,8 +43103,11 @@
       <c r="N289">
         <v>0.73545000000000005</v>
       </c>
-    </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O289">
+        <v>0.73850300000000002</v>
+      </c>
+    </row>
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -42279,8 +43150,11 @@
       <c r="N290">
         <v>1.0185599999999999</v>
       </c>
-    </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O290">
+        <v>1.0066200000000001</v>
+      </c>
+    </row>
+    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -42323,8 +43197,11 @@
       <c r="N291">
         <v>0.62238499999999997</v>
       </c>
-    </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O291">
+        <v>0.62310399999999999</v>
+      </c>
+    </row>
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>291</v>
       </c>
@@ -42363,6 +43240,9 @@
       </c>
       <c r="N292" t="s">
         <v>303</v>
+      </c>
+      <c r="O292" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -54622,7 +55502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EE2C5E-70FF-4F3A-85CC-4A11B0D0C8F6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Memory Pool and refine some codes
</commit_message>
<xml_diff>
--- a/app/result.xlsx
+++ b/app/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QOC\MeshSimplification-Mobile\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58659D2-B3B3-45DB-A77C-9CA9BC490F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA1CFF-7FEF-463F-9FC0-E76656D5EAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37695" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
   <si>
     <t>mesh0</t>
   </si>
@@ -951,6 +951,9 @@
   </si>
   <si>
     <t>Customized Face List</t>
+  </si>
+  <si>
+    <t>Memory Pool</t>
   </si>
 </sst>
 </file>
@@ -29500,10 +29503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O292"/>
+  <dimension ref="A1:P292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G283" workbookViewId="0">
-      <selection activeCell="O293" sqref="O293"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29519,12 +29522,13 @@
     <col min="10" max="10" width="32.140625" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
     <col min="12" max="12" width="28.85546875" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" customWidth="1"/>
     <col min="14" max="14" width="39.140625" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="16" max="16" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -29570,8 +29574,11 @@
       <c r="O1">
         <v>13.876099999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1">
+        <v>13.1738</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -29617,8 +29624,11 @@
       <c r="O2">
         <v>12.868</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>12.1592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -29664,8 +29674,11 @@
       <c r="O3">
         <v>12.3248</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>11.6814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -29711,8 +29724,11 @@
       <c r="O4">
         <v>0.52122800000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0.45567000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -29758,8 +29774,11 @@
       <c r="O5">
         <v>0.74739</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>0.69071899999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -29805,8 +29824,11 @@
       <c r="O6">
         <v>0.41814000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>0.38788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -29852,8 +29874,11 @@
       <c r="O7">
         <v>4.6056E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>4.1422100000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -29899,8 +29924,11 @@
       <c r="O8">
         <v>0.29919000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0.28518399999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -29946,8 +29974,11 @@
       <c r="O9">
         <v>1.22804</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>1.1440699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -29993,8 +30024,11 @@
       <c r="O10">
         <v>0.26332</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0.246891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -30040,8 +30074,11 @@
       <c r="O11">
         <v>0.37726999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0.34879199999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -30087,8 +30124,11 @@
       <c r="O12">
         <v>6.9442100000000007E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>6.5063899999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -30134,8 +30174,11 @@
       <c r="O13">
         <v>3.0199799999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>2.9430499999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -30181,8 +30224,11 @@
       <c r="O14">
         <v>21.510999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>20.2501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -30228,8 +30274,11 @@
       <c r="O15">
         <v>0.23832400000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>0.17635799999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -30275,8 +30324,11 @@
       <c r="O16">
         <v>0.35272199999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>0.32276199999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -30322,8 +30374,11 @@
       <c r="O17">
         <v>0.31260599999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0.29437799999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -30369,8 +30424,11 @@
       <c r="O18">
         <v>0.27892</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0.25875700000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -30416,8 +30474,11 @@
       <c r="O19">
         <v>0.44085200000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0.41721999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -30463,8 +30524,11 @@
       <c r="O20">
         <v>1.36486</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>1.31189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -30510,8 +30574,11 @@
       <c r="O21">
         <v>5.8852000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>5.1952100000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -30557,8 +30624,11 @@
       <c r="O22">
         <v>2.9420000000000002E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>2.6418000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -30604,8 +30674,11 @@
       <c r="O23">
         <v>0.723912</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>0.69078200000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -30651,8 +30724,11 @@
       <c r="O24">
         <v>1.0598700000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>1.00607</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -30698,8 +30774,11 @@
       <c r="O25">
         <v>24.981400000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>24.029</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -30745,8 +30824,11 @@
       <c r="O26">
         <v>0.33716400000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>0.27210600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -30792,8 +30874,11 @@
       <c r="O27">
         <v>0.75381600000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>0.68814699999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -30839,8 +30924,11 @@
       <c r="O28">
         <v>9.0819999999999998E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>8.3376099999999995E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -30886,8 +30974,11 @@
       <c r="O29">
         <v>0.410132</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>0.39501999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -30933,8 +31024,11 @@
       <c r="O30">
         <v>0.49485600000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>0.46028400000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -30980,8 +31074,11 @@
       <c r="O31">
         <v>0.33566000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>0.23472499999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -31027,8 +31124,11 @@
       <c r="O32">
         <v>0.86531499999999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>0.80441600000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -31074,8 +31174,11 @@
       <c r="O33">
         <v>0.35054600000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>0.31701000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -31121,8 +31224,11 @@
       <c r="O34">
         <v>0.18883</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>0.17967</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -31168,8 +31274,11 @@
       <c r="O35">
         <v>1.2817799999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>1.2669900000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -31215,8 +31324,11 @@
       <c r="O36">
         <v>12.419600000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>11.759499999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -31262,8 +31374,11 @@
       <c r="O37">
         <v>1.0431900000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>0.94291899999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -31309,8 +31424,11 @@
       <c r="O38">
         <v>0.97958000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>0.89451999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -31356,8 +31474,11 @@
       <c r="O39">
         <v>0.13858599999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>0.124884</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -31403,8 +31524,11 @@
       <c r="O40">
         <v>1.0052099999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>0.93083000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -31450,8 +31574,11 @@
       <c r="O41">
         <v>0.44911800000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>0.41416999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -31497,8 +31624,11 @@
       <c r="O42">
         <v>0.63450399999999996</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>0.60315099999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -31544,8 +31674,11 @@
       <c r="O43">
         <v>0.55200800000000005</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>0.51580599999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -31591,8 +31724,11 @@
       <c r="O44">
         <v>0.58008800000000005</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>0.54137599999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -31638,8 +31774,11 @@
       <c r="O45">
         <v>0.109916</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <v>0.10281800000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -31685,8 +31824,11 @@
       <c r="O46">
         <v>0.67754999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>0.64704200000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -31732,8 +31874,11 @@
       <c r="O47">
         <v>14.024699999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47">
+        <v>13.376899999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -31779,8 +31924,11 @@
       <c r="O48">
         <v>0.18007000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>0.134132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -31826,8 +31974,11 @@
       <c r="O49">
         <v>0.82930999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <v>0.78462900000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -31873,8 +32024,11 @@
       <c r="O50">
         <v>0.19154399999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50">
+        <v>0.18040800000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -31920,8 +32074,11 @@
       <c r="O51">
         <v>0.25369999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <v>0.23596700000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -31967,8 +32124,11 @@
       <c r="O52">
         <v>1.4693400000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52">
+        <v>1.3813299999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -32014,8 +32174,11 @@
       <c r="O53">
         <v>0.83572000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53">
+        <v>0.77788800000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -32061,8 +32224,11 @@
       <c r="O54">
         <v>0.149868</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P54">
+        <v>0.137936</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -32108,8 +32274,11 @@
       <c r="O55">
         <v>0.69219200000000003</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>0.64852799999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -32155,8 +32324,11 @@
       <c r="O56">
         <v>0.90687499999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P56">
+        <v>0.84526100000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -32202,8 +32374,11 @@
       <c r="O57">
         <v>0.52852600000000005</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P57">
+        <v>0.499498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -32249,8 +32424,11 @@
       <c r="O58">
         <v>12.2249</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P58">
+        <v>11.581099999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -32296,8 +32474,11 @@
       <c r="O59">
         <v>0.13419400000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P59">
+        <v>9.5578099999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -32343,8 +32524,11 @@
       <c r="O60">
         <v>0.21416399999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P60">
+        <v>0.18684999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -32390,8 +32574,11 @@
       <c r="O61">
         <v>0.17844199999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P61">
+        <v>0.165074</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -32437,8 +32624,11 @@
       <c r="O62">
         <v>1.5982700000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P62">
+        <v>1.5762499999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -32484,8 +32674,11 @@
       <c r="O63" s="1">
         <v>1.9999999999999999E-6</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -32531,8 +32724,11 @@
       <c r="O64">
         <v>0.97238400000000003</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P64">
+        <v>0.90926799999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -32578,8 +32774,11 @@
       <c r="O65">
         <v>2.4820199999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P65">
+        <v>2.35473</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -32625,8 +32824,11 @@
       <c r="O66">
         <v>5.6948600000000003</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P66">
+        <v>5.3651</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -32672,8 +32874,11 @@
       <c r="O67">
         <v>0.43070399999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P67">
+        <v>0.39073000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -32719,8 +32924,11 @@
       <c r="O68">
         <v>0.44252000000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P68">
+        <v>0.41625400000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -32766,8 +32974,11 @@
       <c r="O69">
         <v>14.063000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P69">
+        <v>13.3872</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -32813,8 +33024,11 @@
       <c r="O70">
         <v>0.32473400000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P70">
+        <v>0.26865</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -32860,8 +33074,11 @@
       <c r="O71">
         <v>7.5651899999999994E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P71">
+        <v>6.9148200000000007E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -32907,8 +33124,11 @@
       <c r="O72">
         <v>0.21074999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P72">
+        <v>0.188114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -32954,8 +33174,11 @@
       <c r="O73">
         <v>0.18499599999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P73">
+        <v>0.16289999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -33001,8 +33224,11 @@
       <c r="O74">
         <v>0.10051400000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P74">
+        <v>9.2757599999999996E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -33048,8 +33274,11 @@
       <c r="O75">
         <v>0.29346800000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P75">
+        <v>0.27301900000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -33095,8 +33324,11 @@
       <c r="O76">
         <v>0.10758</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P76">
+        <v>9.8034099999999999E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -33142,8 +33374,11 @@
       <c r="O77">
         <v>0.99120799999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P77">
+        <v>0.95942899999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -33189,8 +33424,11 @@
       <c r="O78">
         <v>0.32199</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P78">
+        <v>0.28667100000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -33236,8 +33474,11 @@
       <c r="O79">
         <v>0.2185</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P79">
+        <v>0.20432</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -33283,8 +33524,11 @@
       <c r="O80">
         <v>12.404199999999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P80">
+        <v>11.5848</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -33330,8 +33574,11 @@
       <c r="O81">
         <v>0.173594</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P81">
+        <v>0.13492799999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -33377,8 +33624,11 @@
       <c r="O82">
         <v>0.31773800000000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82">
+        <v>0.28865099999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -33424,8 +33674,11 @@
       <c r="O83">
         <v>0.746286</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P83">
+        <v>0.69088799999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -33471,8 +33724,11 @@
       <c r="O84">
         <v>2.5012500000000002</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P84">
+        <v>2.4295100000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -33518,8 +33774,11 @@
       <c r="O85">
         <v>1.04558</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P85">
+        <v>0.97570599999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -33565,8 +33824,11 @@
       <c r="O86">
         <v>0.88053400000000004</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P86">
+        <v>0.852352</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -33612,8 +33874,11 @@
       <c r="O87">
         <v>5.3029899999999998E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P87">
+        <v>5.0818000000000002E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -33659,8 +33924,11 @@
       <c r="O88">
         <v>4.9032100000000002E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P88">
+        <v>4.3954E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -33706,8 +33974,11 @@
       <c r="O89">
         <v>0.127166</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P89">
+        <v>0.114366</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -33753,8 +34024,11 @@
       <c r="O90">
         <v>5.2711899999999999E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P90">
+        <v>4.75381E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -33800,8 +34074,11 @@
       <c r="O91">
         <v>13.9694</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P91">
+        <v>13.3073</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -33847,8 +34124,11 @@
       <c r="O92">
         <v>0.27334599999999998</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P92">
+        <v>0.22639999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -33894,8 +34174,11 @@
       <c r="O93">
         <v>0.22880600000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P93">
+        <v>0.206515</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -33941,8 +34224,11 @@
       <c r="O94">
         <v>0.16092600000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P94">
+        <v>0.14372199999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -33988,8 +34274,11 @@
       <c r="O95">
         <v>0.43972600000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P95">
+        <v>0.41400399999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -34035,8 +34324,11 @@
       <c r="O96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -34082,8 +34374,11 @@
       <c r="O97">
         <v>0.101344</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P97">
+        <v>8.8974300000000006E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -34129,8 +34424,11 @@
       <c r="O98">
         <v>0.16320799999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P98">
+        <v>0.14840600000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -34176,8 +34474,11 @@
       <c r="O99">
         <v>0.12817999999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P99">
+        <v>0.11794399999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -34223,8 +34524,11 @@
       <c r="O100">
         <v>1.92184</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P100">
+        <v>1.85189</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -34270,8 +34574,11 @@
       <c r="O101">
         <v>0.22658600000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P101">
+        <v>0.20927699999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -34317,8 +34624,11 @@
       <c r="O102">
         <v>12.426500000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P102">
+        <v>11.7965</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -34364,8 +34674,11 @@
       <c r="O103">
         <v>1.7175800000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P103">
+        <v>1.5983499999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -34411,8 +34724,11 @@
       <c r="O104">
         <v>0.53626799999999997</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P104">
+        <v>0.51038799999999995</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -34458,8 +34774,11 @@
       <c r="O105">
         <v>0.50555799999999995</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P105">
+        <v>0.46440199999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -34505,8 +34824,11 @@
       <c r="O106">
         <v>0.13137199999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P106">
+        <v>0.11382399999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -34552,8 +34874,11 @@
       <c r="O107">
         <v>0.48840800000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P107">
+        <v>0.462895</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -34599,8 +34924,11 @@
       <c r="O108">
         <v>5.2901900000000002E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P108">
+        <v>4.8026100000000002E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -34646,8 +34974,11 @@
       <c r="O109">
         <v>5.7050099999999999E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P109">
+        <v>5.3631999999999999E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -34693,8 +35024,11 @@
       <c r="O110">
         <v>0.24846799999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P110">
+        <v>0.232846</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -34740,8 +35074,11 @@
       <c r="O111">
         <v>0.106946</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P111">
+        <v>9.8008100000000001E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -34787,8 +35124,11 @@
       <c r="O112">
         <v>4.9195999999999997E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P112">
+        <v>4.3411900000000003E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -34834,8 +35174,11 @@
       <c r="O113">
         <v>12.247999999999999</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P113">
+        <v>11.625299999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -34881,8 +35224,11 @@
       <c r="O114">
         <v>12.4908</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P114">
+        <v>11.8294</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -34928,8 +35274,11 @@
       <c r="O115">
         <v>0.108552</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P115">
+        <v>7.2385900000000003E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -34975,8 +35324,11 @@
       <c r="O116">
         <v>0.69500200000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P116">
+        <v>0.64048799999999995</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -35022,8 +35374,11 @@
       <c r="O117">
         <v>0.106282</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P117">
+        <v>9.20261E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -35069,8 +35424,11 @@
       <c r="O118">
         <v>0.46706999999999999</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P118">
+        <v>0.42239599999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -35116,8 +35474,11 @@
       <c r="O119">
         <v>0.223582</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P119">
+        <v>0.203073</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -35163,8 +35524,11 @@
       <c r="O120">
         <v>0.167106</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P120">
+        <v>0.15390400000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -35210,8 +35574,11 @@
       <c r="O121">
         <v>1.2547299999999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P121">
+        <v>1.2261500000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -35257,8 +35624,11 @@
       <c r="O122">
         <v>2.07931</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P122">
+        <v>1.96811</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -35304,8 +35674,11 @@
       <c r="O123">
         <v>6.7823700000000002</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P123">
+        <v>6.6862899999999996</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -35351,8 +35724,11 @@
       <c r="O124">
         <v>1.0939300000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P124">
+        <v>1.06823</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -35398,8 +35774,11 @@
       <c r="O125">
         <v>14.102</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P125">
+        <v>13.5341</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -35445,8 +35824,11 @@
       <c r="O126">
         <v>3.2933400000000002</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P126">
+        <v>2.90768</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -35492,8 +35874,11 @@
       <c r="O127">
         <v>9.2964000000000005E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P127">
+        <v>7.13699E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -35539,8 +35924,11 @@
       <c r="O128">
         <v>1.33087</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P128">
+        <v>1.2822100000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -35586,8 +35974,11 @@
       <c r="O129">
         <v>1.2424999999999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P129">
+        <v>1.2229099999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -35633,8 +36024,11 @@
       <c r="O130">
         <v>0.19984199999999999</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P130">
+        <v>0.183114</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -35680,8 +36074,11 @@
       <c r="O131">
         <v>6.0960400000000003</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P131">
+        <v>5.7372699999999996</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -35727,8 +36124,11 @@
       <c r="O132">
         <v>0.53234199999999998</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P132">
+        <v>0.46667799999999998</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -35774,8 +36174,11 @@
       <c r="O133">
         <v>1.5354399999999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P133">
+        <v>1.4505399999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -35821,8 +36224,11 @@
       <c r="O134">
         <v>2.0549300000000001</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P134">
+        <v>1.91496</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -35868,8 +36274,11 @@
       <c r="O135">
         <v>2.9029099999999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P135">
+        <v>2.7846299999999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -35915,8 +36324,11 @@
       <c r="O136">
         <v>7.0724600000000004</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P136">
+        <v>6.6668700000000003</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -35962,8 +36374,11 @@
       <c r="O137">
         <v>5.0257199999999997</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P137">
+        <v>4.6639299999999997</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -36009,8 +36424,11 @@
       <c r="O138">
         <v>2.3527499999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P138">
+        <v>2.1791900000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -36056,8 +36474,11 @@
       <c r="O139">
         <v>17.605499999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P139">
+        <v>16.6386</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -36103,8 +36524,11 @@
       <c r="O140">
         <v>17.006499999999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P140">
+        <v>16.248899999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -36150,8 +36574,11 @@
       <c r="O141">
         <v>1.2553700000000001</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P141">
+        <v>1.1652100000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -36197,8 +36624,11 @@
       <c r="O142">
         <v>2.7590699999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P142">
+        <v>2.5901399999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -36244,8 +36674,11 @@
       <c r="O143">
         <v>2.4819300000000002</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P143">
+        <v>2.2972700000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -36291,8 +36724,11 @@
       <c r="O144">
         <v>0.30197200000000002</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P144">
+        <v>0.28061799999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -36338,8 +36774,11 @@
       <c r="O145">
         <v>2.2483499999999998</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P145">
+        <v>1.74129</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -36385,8 +36824,11 @@
       <c r="O146">
         <v>0.59743199999999996</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P146">
+        <v>0.54872399999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -36432,8 +36874,11 @@
       <c r="O147">
         <v>14.049799999999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P147">
+        <v>13.3552</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -36479,8 +36924,11 @@
       <c r="O148">
         <v>3.9306000000000001</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P148">
+        <v>3.6804600000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -36526,8 +36974,11 @@
       <c r="O149">
         <v>3.2639300000000002</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P149">
+        <v>3.09646</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -36573,8 +37024,11 @@
       <c r="O150">
         <v>5.8413899999999996</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P150">
+        <v>5.5302100000000003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -36620,8 +37074,11 @@
       <c r="O151">
         <v>9.04786</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P151">
+        <v>8.5159500000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -36667,8 +37124,11 @@
       <c r="O152">
         <v>0.45798</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P152">
+        <v>0.42727399999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -36714,8 +37174,11 @@
       <c r="O153">
         <v>1.4278900000000001</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P153">
+        <v>1.2522899999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -36761,8 +37224,11 @@
       <c r="O154">
         <v>1.95828</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P154">
+        <v>1.8662300000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -36808,8 +37274,11 @@
       <c r="O155">
         <v>2.7687400000000002</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P155">
+        <v>2.63096</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -36855,8 +37324,11 @@
       <c r="O156">
         <v>3.84477</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P156">
+        <v>3.6806000000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -36902,8 +37374,11 @@
       <c r="O157">
         <v>10.3461</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P157">
+        <v>9.9804999999999993</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -36949,8 +37424,11 @@
       <c r="O158">
         <v>14.115600000000001</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P158">
+        <v>13.4018</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -36996,8 +37474,11 @@
       <c r="O159">
         <v>2.3236300000000001</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P159">
+        <v>2.1741299999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -37043,8 +37524,11 @@
       <c r="O160">
         <v>0.71516400000000002</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P160">
+        <v>0.67256700000000003</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -37090,8 +37574,11 @@
       <c r="O161">
         <v>1.3506199999999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P161">
+        <v>1.2821400000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -37137,8 +37624,11 @@
       <c r="O162">
         <v>4.1378500000000003</v>
       </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P162">
+        <v>4.0551700000000004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -37184,8 +37674,11 @@
       <c r="O163">
         <v>3.3396499999999998</v>
       </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P163">
+        <v>3.12317</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -37231,8 +37724,11 @@
       <c r="O164">
         <v>0.47976400000000002</v>
       </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P164">
+        <v>0.45011400000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -37278,8 +37774,11 @@
       <c r="O165">
         <v>2.1157499999999998</v>
       </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P165">
+        <v>2.0154700000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -37325,8 +37824,11 @@
       <c r="O166">
         <v>2.3347799999999999</v>
       </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P166">
+        <v>2.19475</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -37372,8 +37874,11 @@
       <c r="O167">
         <v>2.79691</v>
       </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P167">
+        <v>2.63117</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -37419,8 +37924,11 @@
       <c r="O168">
         <v>2.0634600000000001</v>
       </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P168">
+        <v>1.9184099999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -37466,8 +37974,11 @@
       <c r="O169">
         <v>21.6585</v>
       </c>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P169">
+        <v>20.616</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -37513,8 +38024,11 @@
       <c r="O170">
         <v>3.4471500000000002</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P170">
+        <v>3.2854899999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -37560,8 +38074,11 @@
       <c r="O171">
         <v>0.56589999999999996</v>
       </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P171">
+        <v>0.52333399999999997</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -37607,8 +38124,11 @@
       <c r="O172">
         <v>0.47023399999999999</v>
       </c>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P172">
+        <v>0.441222</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -37654,8 +38174,11 @@
       <c r="O173">
         <v>0.74380800000000002</v>
       </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P173">
+        <v>0.69116999999999995</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -37701,8 +38224,11 @@
       <c r="O174">
         <v>1.04765</v>
       </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P174">
+        <v>0.95137000000000005</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -37748,8 +38274,11 @@
       <c r="O175">
         <v>0.454538</v>
       </c>
-    </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P175">
+        <v>0.42348599999999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -37795,8 +38324,11 @@
       <c r="O176">
         <v>2.0946899999999999</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P176">
+        <v>1.99892</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -37842,8 +38374,11 @@
       <c r="O177">
         <v>1.84354</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P177">
+        <v>1.71641</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -37889,8 +38424,11 @@
       <c r="O178">
         <v>1.4044399999999999</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P178">
+        <v>1.3193999999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -37936,8 +38474,11 @@
       <c r="O179">
         <v>2.5284900000000001</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P179">
+        <v>2.44943</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -37983,8 +38524,11 @@
       <c r="O180">
         <v>14.122400000000001</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P180">
+        <v>13.637700000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -38030,8 +38574,11 @@
       <c r="O181">
         <v>1.0304</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P181">
+        <v>0.91562699999999997</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -38077,8 +38624,11 @@
       <c r="O182">
         <v>4.09354</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P182">
+        <v>3.9246400000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -38124,8 +38674,11 @@
       <c r="O183">
         <v>0.82743999999999995</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P183">
+        <v>0.80297799999999997</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -38171,8 +38724,11 @@
       <c r="O184">
         <v>0.25467800000000002</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P184">
+        <v>0.237039</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -38218,8 +38774,11 @@
       <c r="O185">
         <v>0.617448</v>
       </c>
-    </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P185">
+        <v>0.57811800000000002</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -38265,8 +38824,11 @@
       <c r="O186">
         <v>1.9932399999999999</v>
       </c>
-    </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P186">
+        <v>1.88121</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -38312,8 +38874,11 @@
       <c r="O187">
         <v>0.293072</v>
       </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P187">
+        <v>0.26215699999999997</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -38359,8 +38924,11 @@
       <c r="O188">
         <v>2.71793</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P188">
+        <v>2.62418</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -38406,8 +38974,11 @@
       <c r="O189">
         <v>4.9336100000000001E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P189">
+        <v>4.4381999999999998E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -38453,8 +39024,11 @@
       <c r="O190">
         <v>0.26786599999999999</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P190">
+        <v>0.242615</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -38500,8 +39074,11 @@
       <c r="O191">
         <v>14.0105</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P191">
+        <v>13.4382</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -38547,8 +39124,11 @@
       <c r="O192">
         <v>2.8814700000000002</v>
       </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P192">
+        <v>2.7034500000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -38594,8 +39174,11 @@
       <c r="O193">
         <v>1.0015700000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P193">
+        <v>0.91702600000000001</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -38641,8 +39224,11 @@
       <c r="O194">
         <v>0.49092799999999998</v>
       </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P194">
+        <v>0.44708399999999998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -38688,8 +39274,11 @@
       <c r="O195">
         <v>0.54190400000000005</v>
       </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P195">
+        <v>0.49080299999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -38735,8 +39324,11 @@
       <c r="O196">
         <v>1.3410899999999999</v>
       </c>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P196">
+        <v>1.2904</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -38782,8 +39374,11 @@
       <c r="O197">
         <v>0.95962099999999995</v>
       </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P197">
+        <v>0.89770099999999997</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -38829,8 +39424,11 @@
       <c r="O198">
         <v>0.35820000000000002</v>
       </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P198">
+        <v>0.33737</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -38876,8 +39474,11 @@
       <c r="O199">
         <v>3.42971</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P199">
+        <v>3.2964000000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -38923,8 +39524,11 @@
       <c r="O200">
         <v>0.89960899999999999</v>
       </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P200">
+        <v>0.84659399999999996</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -38970,8 +39574,11 @@
       <c r="O201">
         <v>0.68192600000000003</v>
       </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P201">
+        <v>0.637656</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -39017,8 +39624,11 @@
       <c r="O202">
         <v>12.479100000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P202">
+        <v>11.9476</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -39064,8 +39674,11 @@
       <c r="O203">
         <v>0.35122399999999998</v>
       </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P203">
+        <v>0.29530800000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -39111,8 +39724,11 @@
       <c r="O204">
         <v>1.20577</v>
       </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P204">
+        <v>1.1337900000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -39158,8 +39774,11 @@
       <c r="O205">
         <v>0.20741200000000001</v>
       </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P205">
+        <v>0.18531</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -39205,8 +39824,11 @@
       <c r="O206">
         <v>1.3281799999999999</v>
       </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P206">
+        <v>1.2824199999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -39252,8 +39874,11 @@
       <c r="O207">
         <v>0.32007600000000003</v>
       </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P207">
+        <v>0.30072399999999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -39299,8 +39924,11 @@
       <c r="O208">
         <v>0.302458</v>
       </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P208">
+        <v>0.283636</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -39346,8 +39974,11 @@
       <c r="O209">
         <v>1.02668</v>
       </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P209">
+        <v>1.0114799999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -39393,8 +40024,11 @@
       <c r="O210">
         <v>9.1976199999999994E-2</v>
       </c>
-    </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P210">
+        <v>8.7239800000000006E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -39440,8 +40074,11 @@
       <c r="O211">
         <v>3.2234099999999999</v>
       </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P211">
+        <v>3.0654300000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -39487,8 +40124,11 @@
       <c r="O212">
         <v>8.0932000000000004E-2</v>
       </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P212">
+        <v>7.0996000000000004E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -39534,8 +40174,11 @@
       <c r="O213">
         <v>12.6615</v>
       </c>
-    </row>
-    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P213">
+        <v>11.991</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -39581,8 +40224,11 @@
       <c r="O214">
         <v>397.553</v>
       </c>
-    </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P214">
+        <v>381.77</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -39628,8 +40274,11 @@
       <c r="O215">
         <v>13.9443</v>
       </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P215">
+        <v>12.646000000000001</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -39675,8 +40324,11 @@
       <c r="O216">
         <v>12.649800000000001</v>
       </c>
-    </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P216">
+        <v>12.077199999999999</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -39722,8 +40374,11 @@
       <c r="O217">
         <v>12.700699999999999</v>
       </c>
-    </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P217">
+        <v>12.086</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -39769,8 +40424,11 @@
       <c r="O218">
         <v>24.9907</v>
       </c>
-    </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P218">
+        <v>24.127300000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -39816,8 +40474,11 @@
       <c r="O219">
         <v>5.9088500000000002</v>
       </c>
-    </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P219">
+        <v>5.5248600000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -39863,8 +40524,11 @@
       <c r="O220">
         <v>12.377599999999999</v>
       </c>
-    </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P220">
+        <v>11.716200000000001</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -39910,8 +40574,11 @@
       <c r="O221">
         <v>11.1173</v>
       </c>
-    </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P221">
+        <v>10.506600000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -39957,8 +40624,11 @@
       <c r="O222">
         <v>11.068899999999999</v>
       </c>
-    </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P222">
+        <v>10.4978</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -40004,8 +40674,11 @@
       <c r="O223">
         <v>14.453200000000001</v>
       </c>
-    </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P223">
+        <v>13.4495</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -40051,8 +40724,11 @@
       <c r="O224">
         <v>12.451599999999999</v>
       </c>
-    </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P224">
+        <v>11.7804</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -40098,8 +40774,11 @@
       <c r="O225">
         <v>20.4084</v>
       </c>
-    </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P225">
+        <v>19.5625</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -40145,8 +40824,11 @@
       <c r="O226">
         <v>12.3626</v>
       </c>
-    </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P226">
+        <v>11.706300000000001</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -40192,8 +40874,11 @@
       <c r="O227">
         <v>12.358700000000001</v>
       </c>
-    </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P227">
+        <v>11.7233</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -40239,8 +40924,11 @@
       <c r="O228">
         <v>12.779199999999999</v>
       </c>
-    </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P228">
+        <v>12.0884</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -40286,8 +40974,11 @@
       <c r="O229">
         <v>5.8380999999999998</v>
       </c>
-    </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P229">
+        <v>5.4812000000000003</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -40333,8 +41024,11 @@
       <c r="O230">
         <v>30.5307</v>
       </c>
-    </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P230">
+        <v>29.653300000000002</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -40380,8 +41074,11 @@
       <c r="O231">
         <v>30.527000000000001</v>
       </c>
-    </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P231">
+        <v>29.674700000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -40427,8 +41124,11 @@
       <c r="O232">
         <v>12.824999999999999</v>
       </c>
-    </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P232">
+        <v>12.097300000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -40474,8 +41174,11 @@
       <c r="O233">
         <v>2.5759300000000001</v>
       </c>
-    </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P233">
+        <v>2.3789099999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -40521,8 +41224,11 @@
       <c r="O234">
         <v>0.107084</v>
       </c>
-    </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P234">
+        <v>9.5452200000000001E-2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -40568,8 +41274,11 @@
       <c r="O235">
         <v>4.4727900000000001E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P235">
+        <v>4.11621E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -40615,8 +41324,11 @@
       <c r="O236">
         <v>2.12818</v>
       </c>
-    </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P236">
+        <v>2.04881</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -40662,8 +41374,11 @@
       <c r="O237">
         <v>12.269600000000001</v>
       </c>
-    </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P237">
+        <v>11.6371</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -40709,8 +41424,11 @@
       <c r="O238">
         <v>0.65026399999999995</v>
       </c>
-    </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P238">
+        <v>0.59802999999999995</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -40756,8 +41474,11 @@
       <c r="O239">
         <v>1.1966399999999999</v>
       </c>
-    </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P239">
+        <v>1.1597599999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -40803,8 +41524,11 @@
       <c r="O240">
         <v>1.0465199999999999</v>
       </c>
-    </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P240">
+        <v>1.00013</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -40850,8 +41574,11 @@
       <c r="O241">
         <v>0.17752799999999999</v>
       </c>
-    </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P241">
+        <v>0.16212199999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -40897,8 +41624,11 @@
       <c r="O242">
         <v>0.12515999999999999</v>
       </c>
-    </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P242">
+        <v>0.112286</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -40944,8 +41674,11 @@
       <c r="O243">
         <v>0.36576199999999998</v>
       </c>
-    </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P243">
+        <v>0.34408</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -40991,8 +41724,11 @@
       <c r="O244">
         <v>1.82497</v>
       </c>
-    </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P244">
+        <v>1.718</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -41038,8 +41774,11 @@
       <c r="O245">
         <v>1.8306199999999999</v>
       </c>
-    </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P245">
+        <v>1.69346</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -41085,8 +41824,11 @@
       <c r="O246">
         <v>0.115298</v>
       </c>
-    </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P246">
+        <v>0.1021</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -41132,8 +41874,11 @@
       <c r="O247">
         <v>5.2069900000000002E-2</v>
       </c>
-    </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P247">
+        <v>4.8268100000000001E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -41179,8 +41924,11 @@
       <c r="O248">
         <v>12.2264</v>
       </c>
-    </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P248">
+        <v>11.6091</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -41226,8 +41974,11 @@
       <c r="O249">
         <v>1.9612400000000001</v>
       </c>
-    </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P249">
+        <v>1.87137</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -41273,8 +42024,11 @@
       <c r="O250">
         <v>0.16031400000000001</v>
       </c>
-    </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P250">
+        <v>0.14211199999999999</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -41320,8 +42074,11 @@
       <c r="O251">
         <v>2.5624699999999998</v>
       </c>
-    </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P251">
+        <v>2.44333</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -41367,8 +42124,11 @@
       <c r="O252">
         <v>0.16498199999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P252">
+        <v>0.14690400000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -41414,8 +42174,11 @@
       <c r="O253">
         <v>0.84474199999999999</v>
       </c>
-    </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P253">
+        <v>0.78676599999999997</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -41461,8 +42224,11 @@
       <c r="O254">
         <v>23.4407</v>
       </c>
-    </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P254">
+        <v>23.2226</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -41508,8 +42274,11 @@
       <c r="O255">
         <v>1.13181</v>
       </c>
-    </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P255">
+        <v>1.04427</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -41555,8 +42324,11 @@
       <c r="O256">
         <v>0.56054000000000004</v>
       </c>
-    </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P256">
+        <v>0.52674699999999997</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -41602,8 +42374,11 @@
       <c r="O257">
         <v>0.64557799999999999</v>
       </c>
-    </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P257">
+        <v>0.60113499999999997</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -41649,8 +42424,11 @@
       <c r="O258">
         <v>3.0100500000000001</v>
       </c>
-    </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P258">
+        <v>2.8507099999999999</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -41696,8 +42474,11 @@
       <c r="O259">
         <v>25.2437</v>
       </c>
-    </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P259">
+        <v>24.0609</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -41743,8 +42524,11 @@
       <c r="O260">
         <v>1.58134</v>
       </c>
-    </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P260">
+        <v>1.4066000000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -41790,8 +42574,11 @@
       <c r="O261">
         <v>0.64690800000000004</v>
       </c>
-    </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P261">
+        <v>0.59896199999999999</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -41837,8 +42624,11 @@
       <c r="O262">
         <v>0.53674999999999995</v>
       </c>
-    </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P262">
+        <v>0.49450300000000003</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -41884,8 +42674,11 @@
       <c r="O263">
         <v>0.101826</v>
       </c>
-    </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P263">
+        <v>9.0744099999999994E-2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -41931,8 +42724,11 @@
       <c r="O264">
         <v>1.8466800000000001</v>
       </c>
-    </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P264">
+        <v>1.7423599999999999</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -41978,8 +42774,11 @@
       <c r="O265">
         <v>1.0201199999999999</v>
       </c>
-    </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P265">
+        <v>0.99044500000000002</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -42025,8 +42824,11 @@
       <c r="O266">
         <v>0.84428000000000003</v>
       </c>
-    </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P266">
+        <v>0.81148399999999998</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -42072,8 +42874,11 @@
       <c r="O267">
         <v>0.23902799999999999</v>
       </c>
-    </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P267">
+        <v>0.219387</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -42119,8 +42924,11 @@
       <c r="O268">
         <v>1.04199</v>
       </c>
-    </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P268">
+        <v>0.98089099999999996</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -42166,8 +42974,11 @@
       <c r="O269">
         <v>7.8033700000000001</v>
       </c>
-    </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P269">
+        <v>2.2877299999999998</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -42213,8 +43024,11 @@
       <c r="O270">
         <v>12.3081</v>
       </c>
-    </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P270">
+        <v>11.6554</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -42260,8 +43074,11 @@
       <c r="O271">
         <v>1.4857100000000001</v>
       </c>
-    </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P271">
+        <v>1.31725</v>
+      </c>
+    </row>
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -42307,8 +43124,11 @@
       <c r="O272">
         <v>0.85361200000000004</v>
       </c>
-    </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P272">
+        <v>0.82156099999999999</v>
+      </c>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -42354,8 +43174,11 @@
       <c r="O273">
         <v>0.77298800000000001</v>
       </c>
-    </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P273">
+        <v>0.74213399999999996</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -42401,8 +43224,11 @@
       <c r="O274">
         <v>0.54424799999999995</v>
       </c>
-    </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P274">
+        <v>0.52672300000000005</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -42448,8 +43274,11 @@
       <c r="O275">
         <v>5.6062099999999997E-2</v>
       </c>
-    </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P275">
+        <v>5.0525899999999999E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -42495,8 +43324,11 @@
       <c r="O276">
         <v>0.64577399999999996</v>
       </c>
-    </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P276">
+        <v>0.60120200000000001</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -42542,8 +43374,11 @@
       <c r="O277">
         <v>3.6642000000000001</v>
       </c>
-    </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P277">
+        <v>0.88503500000000002</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -42589,8 +43424,11 @@
       <c r="O278">
         <v>0.86591399999999996</v>
       </c>
-    </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P278">
+        <v>0.82533299999999998</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -42636,8 +43474,11 @@
       <c r="O279">
         <v>1.3997999999999999</v>
       </c>
-    </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P279">
+        <v>1.3292600000000001</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -42683,8 +43524,11 @@
       <c r="O280">
         <v>0.63684200000000002</v>
       </c>
-    </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P280">
+        <v>0.59168600000000005</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -42730,8 +43574,11 @@
       <c r="O281">
         <v>13.6343</v>
       </c>
-    </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P281">
+        <v>11.6213</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -42777,8 +43624,11 @@
       <c r="O282">
         <v>0.62165199999999998</v>
       </c>
-    </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P282">
+        <v>0.54128200000000004</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -42824,8 +43674,11 @@
       <c r="O283">
         <v>0.135438</v>
       </c>
-    </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P283">
+        <v>0.121258</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -42871,8 +43724,11 @@
       <c r="O284">
         <v>0.53527000000000002</v>
       </c>
-    </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P284">
+        <v>0.48349599999999998</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -42918,8 +43774,11 @@
       <c r="O285">
         <v>0.48510399999999998</v>
       </c>
-    </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P285">
+        <v>0.44883000000000001</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -42965,8 +43824,11 @@
       <c r="O286">
         <v>0.25875599999999999</v>
       </c>
-    </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P286">
+        <v>0.24008199999999999</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -43012,8 +43874,11 @@
       <c r="O287">
         <v>0.425508</v>
       </c>
-    </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P287">
+        <v>0.411134</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -43059,8 +43924,11 @@
       <c r="O288">
         <v>7.8096100000000002E-2</v>
       </c>
-    </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P288">
+        <v>7.1131899999999998E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -43106,8 +43974,11 @@
       <c r="O289">
         <v>0.67880399999999996</v>
       </c>
-    </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P289">
+        <v>0.655976</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -43153,8 +44024,11 @@
       <c r="O290">
         <v>0.94694800000000001</v>
       </c>
-    </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P290">
+        <v>0.94132899999999997</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -43200,8 +44074,11 @@
       <c r="O291">
         <v>0.56803000000000003</v>
       </c>
-    </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P291">
+        <v>0.53643600000000002</v>
+      </c>
+    </row>
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>291</v>
       </c>
@@ -43243,6 +44120,9 @@
       </c>
       <c r="O292" t="s">
         <v>304</v>
+      </c>
+      <c r="P292" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove face node pool
</commit_message>
<xml_diff>
--- a/app/result.xlsx
+++ b/app/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QOC\MeshSimplification-Mobile\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FD632A-CBD3-4A3A-B5FE-37973DC633A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A2453D-098A-436F-A59E-5DB0DCDABA25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>mesh0</t>
   </si>
@@ -957,6 +957,9 @@
   </si>
   <si>
     <t>Clear some memory pool</t>
+  </si>
+  <si>
+    <t>Remove face node pool</t>
   </si>
 </sst>
 </file>
@@ -29506,10 +29509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q292"/>
+  <dimension ref="A1:R292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L277" workbookViewId="0">
-      <selection activeCell="Q293" sqref="Q293"/>
+    <sheetView tabSelected="1" topLeftCell="L255" workbookViewId="0">
+      <selection activeCell="R292" sqref="R292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29530,9 +29533,10 @@
     <col min="15" max="15" width="30" customWidth="1"/>
     <col min="16" max="16" width="34.5703125" customWidth="1"/>
     <col min="17" max="17" width="28.28515625" customWidth="1"/>
+    <col min="18" max="18" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -29584,8 +29588,11 @@
       <c r="Q1">
         <v>12.991</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1">
+        <v>12.9941</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -29637,8 +29644,11 @@
       <c r="Q2">
         <v>12.043100000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>12.010199999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -29690,8 +29700,11 @@
       <c r="Q3">
         <v>11.5776</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>11.5533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -29743,8 +29756,11 @@
       <c r="Q4">
         <v>0.45149</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>0.45411600000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -29796,8 +29812,11 @@
       <c r="Q5">
         <v>0.67437000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0.68189599999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -29849,8 +29868,11 @@
       <c r="Q6">
         <v>0.37579000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>0.380886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -29902,8 +29924,11 @@
       <c r="Q7">
         <v>3.9742E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>3.9732000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -29955,8 +29980,11 @@
       <c r="Q8">
         <v>0.276561</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>0.27764299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -30008,8 +30036,11 @@
       <c r="Q9">
         <v>1.12358</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>1.1208100000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -30061,8 +30092,11 @@
       <c r="Q10">
         <v>0.241893</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>0.241593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -30114,8 +30148,11 @@
       <c r="Q11">
         <v>0.34666799999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0.34359000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -30167,8 +30204,11 @@
       <c r="Q12">
         <v>6.3725900000000002E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>6.3477800000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -30220,8 +30260,11 @@
       <c r="Q13">
         <v>2.9515600000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>2.9862899999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -30273,8 +30316,11 @@
       <c r="Q14">
         <v>20.064</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>20.0305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -30326,8 +30372,11 @@
       <c r="Q15">
         <v>0.17711399999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>0.178344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -30379,8 +30428,11 @@
       <c r="Q16">
         <v>0.32405499999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0.32240600000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -30432,8 +30484,11 @@
       <c r="Q17">
         <v>0.291659</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>0.292215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -30485,8 +30540,11 @@
       <c r="Q18">
         <v>0.25703900000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>0.25391799999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -30538,8 +30596,11 @@
       <c r="Q19">
         <v>0.41562199999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>0.41084799999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -30591,8 +30652,11 @@
       <c r="Q20">
         <v>1.3009599999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>1.3025800000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -30644,8 +30708,11 @@
       <c r="Q21">
         <v>5.1692000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>5.1381900000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -30697,8 +30764,11 @@
       <c r="Q22">
         <v>2.5647900000000001E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>2.6450000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -30750,8 +30820,11 @@
       <c r="Q23">
         <v>0.67386199999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>0.68499600000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -30803,8 +30876,11 @@
       <c r="Q24">
         <v>0.97484000000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>0.98772700000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -30856,8 +30932,11 @@
       <c r="Q25">
         <v>23.8687</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>23.716899999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -30909,8 +30988,11 @@
       <c r="Q26">
         <v>0.269374</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>0.269924</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -30962,8 +31044,11 @@
       <c r="Q27">
         <v>0.678894</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>0.680786</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -31015,8 +31100,11 @@
       <c r="Q28">
         <v>7.9133800000000004E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>7.9507999999999995E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -31068,8 +31156,11 @@
       <c r="Q29">
         <v>0.38658599999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>0.388152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -31121,8 +31212,11 @@
       <c r="Q30">
         <v>0.45898600000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>0.456036</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -31174,8 +31268,11 @@
       <c r="Q31">
         <v>0.23285500000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>0.23325499999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -31227,8 +31324,11 @@
       <c r="Q32">
         <v>0.799126</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>0.79718299999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -31280,8 +31380,11 @@
       <c r="Q33">
         <v>0.31581599999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>0.31515599999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -31333,8 +31436,11 @@
       <c r="Q34">
         <v>0.17680799999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>0.17623</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -31386,8 +31492,11 @@
       <c r="Q35">
         <v>1.26109</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>1.2645</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -31439,8 +31548,11 @@
       <c r="Q36">
         <v>11.587999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>11.5829</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -31492,8 +31604,11 @@
       <c r="Q37">
         <v>0.92493199999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <v>0.92711399999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -31545,8 +31660,11 @@
       <c r="Q38">
         <v>0.88268199999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>0.88602999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -31598,8 +31716,11 @@
       <c r="Q39">
         <v>0.124574</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>0.123918</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -31651,8 +31772,11 @@
       <c r="Q40">
         <v>0.92179299999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>0.91572600000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -31704,8 +31828,11 @@
       <c r="Q41">
         <v>0.40573399999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>0.40534799999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -31757,8 +31884,11 @@
       <c r="Q42">
         <v>0.590754</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>0.59093799999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -31810,8 +31940,11 @@
       <c r="Q43">
         <v>0.50421000000000005</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>0.50740399999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -31863,8 +31996,11 @@
       <c r="Q44">
         <v>0.52833600000000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>0.52785199999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -31916,8 +32052,11 @@
       <c r="Q45">
         <v>0.101504</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>0.101646</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -31969,8 +32108,11 @@
       <c r="Q46">
         <v>0.64320999999999995</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>0.64636199999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -32022,8 +32164,11 @@
       <c r="Q47">
         <v>13.1928</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>13.2013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -32075,8 +32220,11 @@
       <c r="Q48">
         <v>0.13262199999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>0.135294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -32128,8 +32276,11 @@
       <c r="Q49">
         <v>0.76101700000000005</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>0.77225600000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -32181,8 +32332,11 @@
       <c r="Q50">
         <v>0.176314</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>0.177236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -32234,8 +32388,11 @@
       <c r="Q51">
         <v>0.23158300000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>0.23278599999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -32287,8 +32444,11 @@
       <c r="Q52">
         <v>1.36114</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52">
+        <v>1.3652200000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -32340,8 +32500,11 @@
       <c r="Q53">
         <v>0.77435399999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53">
+        <v>0.76982799999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -32393,8 +32556,11 @@
       <c r="Q54">
         <v>0.13639399999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54">
+        <v>0.13621</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -32446,8 +32612,11 @@
       <c r="Q55">
         <v>0.64227599999999996</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55">
+        <v>0.64403900000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -32499,8 +32668,11 @@
       <c r="Q56">
         <v>0.83016000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56">
+        <v>0.82688499999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -32552,8 +32724,11 @@
       <c r="Q57">
         <v>0.48516399999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57">
+        <v>0.48764400000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -32605,8 +32780,11 @@
       <c r="Q58">
         <v>11.4472</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58">
+        <v>11.422599999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -32658,8 +32836,11 @@
       <c r="Q59">
         <v>9.4498100000000002E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R59">
+        <v>9.4198000000000004E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -32711,8 +32892,11 @@
       <c r="Q60">
         <v>0.184472</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60">
+        <v>0.18548300000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -32764,8 +32948,11 @@
       <c r="Q61">
         <v>0.163216</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <v>0.16131000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -32817,8 +33004,11 @@
       <c r="Q62">
         <v>1.5758799999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>1.5861799999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -32870,8 +33060,11 @@
       <c r="Q63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -32923,8 +33116,11 @@
       <c r="Q64">
         <v>0.89285400000000004</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R64">
+        <v>0.89640699999999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -32976,8 +33172,11 @@
       <c r="Q65">
         <v>2.3089499999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R65">
+        <v>2.32043</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -33029,8 +33228,11 @@
       <c r="Q66">
         <v>5.3223599999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R66">
+        <v>5.3035100000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -33082,8 +33284,11 @@
       <c r="Q67">
         <v>0.38648199999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R67">
+        <v>0.38508199999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -33135,8 +33340,11 @@
       <c r="Q68">
         <v>0.41326800000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R68">
+        <v>0.40946399999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -33188,8 +33396,11 @@
       <c r="Q69">
         <v>13.201700000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <v>13.2385</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -33241,8 +33452,11 @@
       <c r="Q70">
         <v>0.26575599999999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <v>0.26602199999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -33294,8 +33508,11 @@
       <c r="Q71">
         <v>6.8784200000000004E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R71">
+        <v>6.6982E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -33347,8 +33564,11 @@
       <c r="Q72">
         <v>0.18684700000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R72">
+        <v>0.18645100000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -33400,8 +33620,11 @@
       <c r="Q73">
         <v>0.15906200000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R73">
+        <v>0.16010199999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -33453,8 +33676,11 @@
       <c r="Q74">
         <v>9.36197E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <v>9.3203800000000003E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -33506,8 +33732,11 @@
       <c r="Q75">
         <v>0.27275100000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <v>0.27148699999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -33559,8 +33788,11 @@
       <c r="Q76">
         <v>9.7720299999999996E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <v>9.74603E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -33612,8 +33844,11 @@
       <c r="Q77">
         <v>0.950654</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R77">
+        <v>0.94944200000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -33665,8 +33900,11 @@
       <c r="Q78">
         <v>0.28261799999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R78">
+        <v>0.28083999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -33718,8 +33956,11 @@
       <c r="Q79">
         <v>0.20089499999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R79">
+        <v>0.20032800000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -33771,8 +34012,11 @@
       <c r="Q80">
         <v>11.432</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R80">
+        <v>11.4152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -33824,8 +34068,11 @@
       <c r="Q81">
         <v>0.13450200000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R81">
+        <v>0.133658</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -33877,8 +34124,11 @@
       <c r="Q82">
         <v>0.28722599999999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R82">
+        <v>0.28906599999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -33930,8 +34180,11 @@
       <c r="Q83">
         <v>0.68208599999999997</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R83">
+        <v>0.68398599999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -33983,8 +34236,11 @@
       <c r="Q84">
         <v>2.3887999999999998</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R84">
+        <v>2.3893399999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -34036,8 +34292,11 @@
       <c r="Q85">
         <v>0.94633199999999995</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R85">
+        <v>0.95316400000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -34089,8 +34348,11 @@
       <c r="Q86">
         <v>0.84641</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R86">
+        <v>0.86970800000000004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -34142,8 +34404,11 @@
       <c r="Q87">
         <v>4.8652000000000001E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R87">
+        <v>4.9189999999999998E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -34195,8 +34460,11 @@
       <c r="Q88">
         <v>4.3093899999999997E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R88">
+        <v>4.3121899999999998E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -34248,8 +34516,11 @@
       <c r="Q89">
         <v>0.113612</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <v>0.112788</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -34301,8 +34572,11 @@
       <c r="Q90">
         <v>4.57539E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R90">
+        <v>4.5969999999999997E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -34354,8 +34628,11 @@
       <c r="Q91">
         <v>13.1442</v>
       </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R91">
+        <v>13.141299999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -34407,8 +34684,11 @@
       <c r="Q92">
         <v>0.221197</v>
       </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R92">
+        <v>0.220026</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -34460,8 +34740,11 @@
       <c r="Q93">
         <v>0.20414599999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R93">
+        <v>0.20307600000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -34513,8 +34796,11 @@
       <c r="Q94">
         <v>0.13974200000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R94">
+        <v>0.14095199999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -34566,8 +34852,11 @@
       <c r="Q95">
         <v>0.40577600000000003</v>
       </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R95">
+        <v>0.412636</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -34619,8 +34908,11 @@
       <c r="Q96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -34672,8 +34964,11 @@
       <c r="Q97">
         <v>8.8170200000000004E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R97">
+        <v>8.75441E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -34725,8 +35020,11 @@
       <c r="Q98">
         <v>5.6627900000000002E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R98">
+        <v>5.5432200000000001E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -34778,8 +35076,11 @@
       <c r="Q99">
         <v>0.117372</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R99">
+        <v>0.115924</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -34831,8 +35132,11 @@
       <c r="Q100">
         <v>1.82657</v>
       </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R100">
+        <v>1.8333299999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -34884,8 +35188,11 @@
       <c r="Q101">
         <v>0.206039</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R101">
+        <v>0.206155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -34937,8 +35244,11 @@
       <c r="Q102">
         <v>11.6318</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R102">
+        <v>11.6158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -34990,8 +35300,11 @@
       <c r="Q103">
         <v>1.57165</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R103">
+        <v>1.58195</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -35043,8 +35356,11 @@
       <c r="Q104">
         <v>0.50063800000000003</v>
       </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R104">
+        <v>0.50361400000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -35096,8 +35412,11 @@
       <c r="Q105">
         <v>0.460316</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R105">
+        <v>0.460758</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -35149,8 +35468,11 @@
       <c r="Q106">
         <v>0.11208</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R106">
+        <v>0.11357200000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -35202,8 +35524,11 @@
       <c r="Q107">
         <v>0.45902799999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R107">
+        <v>0.45751999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -35255,8 +35580,11 @@
       <c r="Q108">
         <v>4.6713900000000003E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R108">
+        <v>4.6761900000000002E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -35308,8 +35636,11 @@
       <c r="Q109">
         <v>5.2526000000000003E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R109">
+        <v>5.2044100000000003E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -35361,8 +35692,11 @@
       <c r="Q110">
         <v>0.229407</v>
       </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R110">
+        <v>0.22736899999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -35414,8 +35748,11 @@
       <c r="Q111">
         <v>9.6452300000000005E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R111">
+        <v>9.5490400000000003E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -35467,8 +35804,11 @@
       <c r="Q112">
         <v>4.2659900000000001E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R112">
+        <v>4.22219E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -35520,8 +35860,11 @@
       <c r="Q113">
         <v>11.4803</v>
       </c>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R113">
+        <v>11.451000000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -35573,8 +35916,11 @@
       <c r="Q114">
         <v>11.708399999999999</v>
       </c>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R114">
+        <v>11.6873</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -35626,8 +35972,11 @@
       <c r="Q115">
         <v>7.3251899999999995E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R115">
+        <v>7.2655899999999995E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -35679,8 +36028,11 @@
       <c r="Q116">
         <v>0.62956400000000001</v>
       </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R116">
+        <v>0.63197400000000004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -35732,8 +36084,11 @@
       <c r="Q117">
         <v>4.2737999999999998E-2</v>
       </c>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R117">
+        <v>4.2313999999999997E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -35785,8 +36140,11 @@
       <c r="Q118">
         <v>0.41533599999999998</v>
       </c>
-    </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R118">
+        <v>0.41536600000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -35838,8 +36196,11 @@
       <c r="Q119">
         <v>0.20008400000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R119">
+        <v>0.20150699999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -35891,8 +36252,11 @@
       <c r="Q120">
         <v>0.14943400000000001</v>
       </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R120">
+        <v>0.147532</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -35944,8 +36308,11 @@
       <c r="Q121">
         <v>1.2044900000000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R121">
+        <v>1.20408</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -35997,8 +36364,11 @@
       <c r="Q122">
         <v>1.9329400000000001</v>
       </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R122">
+        <v>1.9432100000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -36050,8 +36420,11 @@
       <c r="Q123">
         <v>6.6836799999999998</v>
       </c>
-    </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R123">
+        <v>6.8239599999999996</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -36103,8 +36476,11 @@
       <c r="Q124">
         <v>1.0465500000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R124">
+        <v>1.0466</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -36156,8 +36532,11 @@
       <c r="Q125">
         <v>13.3161</v>
       </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R125">
+        <v>13.3178</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -36209,8 +36588,11 @@
       <c r="Q126">
         <v>2.9067599999999998</v>
       </c>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R126">
+        <v>2.8738999999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -36262,8 +36644,11 @@
       <c r="Q127">
         <v>6.9774000000000003E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R127">
+        <v>7.3053900000000005E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -36315,8 +36700,11 @@
       <c r="Q128">
         <v>1.2682100000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R128">
+        <v>1.27965</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -36368,8 +36756,11 @@
       <c r="Q129">
         <v>1.2010700000000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R129">
+        <v>1.20136</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -36421,8 +36812,11 @@
       <c r="Q130">
         <v>0.180006</v>
       </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R130">
+        <v>0.17737600000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -36474,8 +36868,11 @@
       <c r="Q131">
         <v>5.6708800000000004</v>
       </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R131">
+        <v>5.6639099999999996</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -36527,8 +36924,11 @@
       <c r="Q132">
         <v>0.45869799999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R132">
+        <v>0.45982600000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -36580,8 +36980,11 @@
       <c r="Q133">
         <v>1.4349099999999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R133">
+        <v>1.4303699999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -36633,8 +37036,11 @@
       <c r="Q134">
         <v>1.89134</v>
       </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R134">
+        <v>1.8933</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -36686,8 +37092,11 @@
       <c r="Q135">
         <v>2.7390699999999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R135">
+        <v>2.7494000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -36739,8 +37148,11 @@
       <c r="Q136">
         <v>6.5696399999999997</v>
       </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R136">
+        <v>6.6059900000000003</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -36792,8 +37204,11 @@
       <c r="Q137">
         <v>4.6216799999999996</v>
       </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R137">
+        <v>4.6240600000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -36845,8 +37260,11 @@
       <c r="Q138">
         <v>2.1525099999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R138">
+        <v>2.1492200000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -36898,8 +37316,11 @@
       <c r="Q139">
         <v>16.450399999999998</v>
       </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R139">
+        <v>16.434200000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -36951,8 +37372,11 @@
       <c r="Q140">
         <v>16.088200000000001</v>
       </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R140">
+        <v>16.0777</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -37004,8 +37428,11 @@
       <c r="Q141">
         <v>1.14802</v>
       </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R141">
+        <v>1.13845</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -37057,8 +37484,11 @@
       <c r="Q142">
         <v>2.5539399999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R142">
+        <v>2.55071</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -37110,8 +37540,11 @@
       <c r="Q143">
         <v>2.2701899999999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R143">
+        <v>2.2884600000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -37163,8 +37596,11 @@
       <c r="Q144">
         <v>0.27491700000000002</v>
       </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R144">
+        <v>0.27660699999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -37216,8 +37652,11 @@
       <c r="Q145">
         <v>1.7227600000000001</v>
       </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R145">
+        <v>1.7174</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -37269,8 +37708,11 @@
       <c r="Q146">
         <v>0.54251000000000005</v>
       </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R146">
+        <v>0.53888800000000003</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -37322,8 +37764,11 @@
       <c r="Q147">
         <v>13.1845</v>
       </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R147">
+        <v>13.191000000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -37375,8 +37820,11 @@
       <c r="Q148">
         <v>3.6446900000000002</v>
       </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R148">
+        <v>3.6489099999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -37428,8 +37876,11 @@
       <c r="Q149">
         <v>3.0525000000000002</v>
       </c>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R149">
+        <v>3.0533800000000002</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -37481,8 +37932,11 @@
       <c r="Q150">
         <v>5.4561099999999998</v>
       </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R150">
+        <v>5.4567100000000002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -37534,8 +37988,11 @@
       <c r="Q151">
         <v>8.4282599999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R151">
+        <v>8.4269999999999996</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -37587,8 +38044,11 @@
       <c r="Q152">
         <v>0.42016799999999999</v>
       </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R152">
+        <v>0.41899399999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -37640,8 +38100,11 @@
       <c r="Q153">
         <v>1.2355499999999999</v>
       </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R153">
+        <v>1.2273799999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -37693,8 +38156,11 @@
       <c r="Q154">
         <v>1.8382700000000001</v>
       </c>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R154">
+        <v>1.8501099999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -37746,8 +38212,11 @@
       <c r="Q155">
         <v>2.5957400000000002</v>
       </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R155">
+        <v>2.5954600000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -37799,8 +38268,11 @@
       <c r="Q156">
         <v>3.62324</v>
       </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R156">
+        <v>3.6220599999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -37852,8 +38324,11 @@
       <c r="Q157">
         <v>9.8506900000000002</v>
       </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R157">
+        <v>9.8822399999999995</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -37905,8 +38380,11 @@
       <c r="Q158">
         <v>13.2311</v>
       </c>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R158">
+        <v>13.2578</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -37958,8 +38436,11 @@
       <c r="Q159">
         <v>2.1416400000000002</v>
       </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R159">
+        <v>2.1438799999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -38011,8 +38492,11 @@
       <c r="Q160">
         <v>0.66254000000000002</v>
       </c>
-    </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R160">
+        <v>0.66437100000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -38064,8 +38548,11 @@
       <c r="Q161">
         <v>1.25407</v>
       </c>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R161">
+        <v>1.2537400000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -38117,8 +38604,11 @@
       <c r="Q162">
         <v>3.9969000000000001</v>
       </c>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R162">
+        <v>3.9949300000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -38170,8 +38660,11 @@
       <c r="Q163">
         <v>3.0829499999999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R163">
+        <v>3.10378</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -38223,8 +38716,11 @@
       <c r="Q164">
         <v>0.44385999999999998</v>
       </c>
-    </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R164">
+        <v>0.44406200000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -38276,8 +38772,11 @@
       <c r="Q165">
         <v>1.98434</v>
       </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R165">
+        <v>1.98508</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -38329,8 +38828,11 @@
       <c r="Q166">
         <v>2.16181</v>
       </c>
-    </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R166">
+        <v>2.1694300000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -38382,8 +38884,11 @@
       <c r="Q167">
         <v>2.5915400000000002</v>
       </c>
-    </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R167">
+        <v>2.6019000000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -38435,8 +38940,11 @@
       <c r="Q168">
         <v>1.88673</v>
       </c>
-    </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R168">
+        <v>1.9155</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -38488,8 +38996,11 @@
       <c r="Q169">
         <v>20.2896</v>
       </c>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R169">
+        <v>20.462900000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -38541,8 +39052,11 @@
       <c r="Q170">
         <v>3.2384900000000001</v>
       </c>
-    </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R170">
+        <v>3.2399499999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -38594,8 +39108,11 @@
       <c r="Q171">
         <v>0.50769600000000004</v>
       </c>
-    </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R171">
+        <v>0.51458999999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -38647,8 +39164,11 @@
       <c r="Q172">
         <v>0.43549599999999999</v>
       </c>
-    </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R172">
+        <v>0.43702600000000003</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -38700,8 +39220,11 @@
       <c r="Q173">
         <v>0.68117399999999995</v>
       </c>
-    </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R173">
+        <v>0.67847199999999996</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -38753,8 +39276,11 @@
       <c r="Q174">
         <v>0.939473</v>
       </c>
-    </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R174">
+        <v>0.936554</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -38806,8 +39332,11 @@
       <c r="Q175">
         <v>0.42079</v>
       </c>
-    </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R175">
+        <v>0.41694199999999998</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -38859,8 +39388,11 @@
       <c r="Q176">
         <v>1.97394</v>
       </c>
-    </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R176">
+        <v>1.9768699999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -38912,8 +39444,11 @@
       <c r="Q177">
         <v>1.6904999999999999</v>
       </c>
-    </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R177">
+        <v>1.6933499999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -38965,8 +39500,11 @@
       <c r="Q178">
         <v>1.2969599999999999</v>
       </c>
-    </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R178">
+        <v>1.2989299999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -39018,8 +39556,11 @@
       <c r="Q179">
         <v>2.3956900000000001</v>
       </c>
-    </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R179">
+        <v>2.4015499999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -39071,8 +39612,11 @@
       <c r="Q180">
         <v>13.400700000000001</v>
       </c>
-    </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R180">
+        <v>13.403499999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -39124,8 +39668,11 @@
       <c r="Q181">
         <v>0.90356199999999998</v>
       </c>
-    </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R181">
+        <v>0.90639400000000003</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -39177,8 +39724,11 @@
       <c r="Q182">
         <v>3.8763999999999998</v>
       </c>
-    </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R182">
+        <v>3.8848199999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -39230,8 +39780,11 @@
       <c r="Q183">
         <v>0.78013999999999994</v>
       </c>
-    </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R183">
+        <v>0.786026</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -39283,8 +39836,11 @@
       <c r="Q184">
         <v>0.23110600000000001</v>
       </c>
-    </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R184">
+        <v>0.233546</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -39336,8 +39892,11 @@
       <c r="Q185">
         <v>0.56785600000000003</v>
       </c>
-    </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R185">
+        <v>0.57002600000000003</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -39389,8 +39948,11 @@
       <c r="Q186">
         <v>1.8576900000000001</v>
       </c>
-    </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R186">
+        <v>1.8571299999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -39442,8 +40004,11 @@
       <c r="Q187">
         <v>0.256359</v>
       </c>
-    </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R187">
+        <v>0.25857799999999997</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -39495,8 +40060,11 @@
       <c r="Q188">
         <v>2.5891000000000002</v>
       </c>
-    </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R188">
+        <v>2.5956100000000002</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -39548,8 +40116,11 @@
       <c r="Q189">
         <v>4.5184000000000002E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R189">
+        <v>4.5650000000000003E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -39601,8 +40172,11 @@
       <c r="Q190">
         <v>0.240208</v>
       </c>
-    </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R190">
+        <v>0.24129400000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -39654,8 +40228,11 @@
       <c r="Q191">
         <v>13.2537</v>
       </c>
-    </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R191">
+        <v>13.260899999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -39707,8 +40284,11 @@
       <c r="Q192">
         <v>2.66818</v>
       </c>
-    </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R192">
+        <v>2.6691400000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -39760,8 +40340,11 @@
       <c r="Q193">
         <v>0.89954800000000001</v>
       </c>
-    </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R193">
+        <v>0.89840200000000003</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -39813,8 +40396,11 @@
       <c r="Q194">
         <v>0.437282</v>
       </c>
-    </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R194">
+        <v>0.43784800000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -39866,8 +40452,11 @@
       <c r="Q195">
         <v>0.487896</v>
       </c>
-    </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R195">
+        <v>0.48777599999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -39919,8 +40508,11 @@
       <c r="Q196">
         <v>1.2703</v>
       </c>
-    </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R196">
+        <v>1.27742</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -39972,8 +40564,11 @@
       <c r="Q197">
         <v>0.88801699999999995</v>
       </c>
-    </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R197">
+        <v>0.89072899999999999</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -40025,8 +40620,11 @@
       <c r="Q198">
         <v>0.33088400000000001</v>
       </c>
-    </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R198">
+        <v>0.33306999999999998</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -40078,8 +40676,11 @@
       <c r="Q199">
         <v>3.2407400000000002</v>
       </c>
-    </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R199">
+        <v>3.24525</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -40131,8 +40732,11 @@
       <c r="Q200">
         <v>0.82510799999999995</v>
       </c>
-    </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R200">
+        <v>0.82926200000000005</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -40184,8 +40788,11 @@
       <c r="Q201">
         <v>0.62561800000000001</v>
       </c>
-    </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R201">
+        <v>0.62899400000000005</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -40237,8 +40844,11 @@
       <c r="Q202">
         <v>11.733700000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R202">
+        <v>11.700699999999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -40290,8 +40900,11 @@
       <c r="Q203">
         <v>0.29167999999999999</v>
       </c>
-    </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R203">
+        <v>0.29216399999999998</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -40343,8 +40956,11 @@
       <c r="Q204">
         <v>1.1261699999999999</v>
       </c>
-    </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R204">
+        <v>1.1194200000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -40396,8 +41012,11 @@
       <c r="Q205">
         <v>0.179978</v>
       </c>
-    </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R205">
+        <v>0.182116</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -40449,8 +41068,11 @@
       <c r="Q206">
         <v>1.2643</v>
       </c>
-    </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R206">
+        <v>1.2724899999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -40502,8 +41124,11 @@
       <c r="Q207">
         <v>0.29575400000000002</v>
       </c>
-    </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R207">
+        <v>0.29537200000000002</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -40555,8 +41180,11 @@
       <c r="Q208">
         <v>0.276445</v>
       </c>
-    </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R208">
+        <v>0.280499</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -40608,8 +41236,11 @@
       <c r="Q209">
         <v>0.98754399999999998</v>
       </c>
-    </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R209">
+        <v>1.0015499999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -40661,8 +41292,11 @@
       <c r="Q210">
         <v>8.4957699999999997E-2</v>
       </c>
-    </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R210">
+        <v>8.6455799999999999E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -40714,8 +41348,11 @@
       <c r="Q211">
         <v>3.0280800000000001</v>
       </c>
-    </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R211">
+        <v>3.02366</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -40767,8 +41404,11 @@
       <c r="Q212">
         <v>7.0072099999999998E-2</v>
       </c>
-    </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R212">
+        <v>6.9876099999999997E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -40820,8 +41460,11 @@
       <c r="Q213">
         <v>11.8407</v>
       </c>
-    </row>
-    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R213">
+        <v>11.8286</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -40873,8 +41516,11 @@
       <c r="Q214">
         <v>379.79199999999997</v>
       </c>
-    </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R214">
+        <v>367.10399999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -40926,8 +41572,11 @@
       <c r="Q215">
         <v>12.5501</v>
       </c>
-    </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R215">
+        <v>12.5261</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -40979,8 +41628,11 @@
       <c r="Q216">
         <v>11.9444</v>
       </c>
-    </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R216">
+        <v>11.9147</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -41032,8 +41684,11 @@
       <c r="Q217">
         <v>11.979200000000001</v>
       </c>
-    </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R217">
+        <v>11.945399999999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -41085,8 +41740,11 @@
       <c r="Q218">
         <v>23.9434</v>
       </c>
-    </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R218">
+        <v>23.844999999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -41138,8 +41796,11 @@
       <c r="Q219">
         <v>5.47126</v>
       </c>
-    </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R219">
+        <v>5.4339599999999999</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -41191,8 +41852,11 @@
       <c r="Q220">
         <v>11.580299999999999</v>
       </c>
-    </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R220">
+        <v>11.5801</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -41244,8 +41908,11 @@
       <c r="Q221">
         <v>10.3963</v>
       </c>
-    </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R221">
+        <v>10.3941</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -41297,8 +41964,11 @@
       <c r="Q222">
         <v>10.3843</v>
       </c>
-    </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R222">
+        <v>10.3863</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -41350,8 +42020,11 @@
       <c r="Q223">
         <v>13.306100000000001</v>
       </c>
-    </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R223">
+        <v>13.290699999999999</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -41403,8 +42076,11 @@
       <c r="Q224">
         <v>11.646699999999999</v>
       </c>
-    </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R224">
+        <v>11.6302</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -41456,8 +42132,11 @@
       <c r="Q225">
         <v>19.384399999999999</v>
       </c>
-    </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R225">
+        <v>19.328499999999998</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -41509,8 +42188,11 @@
       <c r="Q226">
         <v>11.591200000000001</v>
       </c>
-    </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R226">
+        <v>11.558999999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -41562,8 +42244,11 @@
       <c r="Q227">
         <v>11.6182</v>
       </c>
-    </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R227">
+        <v>11.582700000000001</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -41615,8 +42300,11 @@
       <c r="Q228">
         <v>11.961399999999999</v>
       </c>
-    </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R228">
+        <v>11.936299999999999</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -41668,8 +42356,11 @@
       <c r="Q229">
         <v>5.41601</v>
       </c>
-    </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R229">
+        <v>5.3997900000000003</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -41721,8 +42412,11 @@
       <c r="Q230">
         <v>29.3355</v>
       </c>
-    </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R230">
+        <v>29.2681</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -41774,8 +42468,11 @@
       <c r="Q231">
         <v>29.3735</v>
       </c>
-    </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R231">
+        <v>29.317900000000002</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -41827,8 +42524,11 @@
       <c r="Q232">
         <v>11.9764</v>
       </c>
-    </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R232">
+        <v>11.948700000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -41880,8 +42580,11 @@
       <c r="Q233">
         <v>2.3778899999999998</v>
       </c>
-    </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R233">
+        <v>2.3511000000000002</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -41933,8 +42636,11 @@
       <c r="Q234">
         <v>9.5023999999999997E-2</v>
       </c>
-    </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R234">
+        <v>9.5002000000000003E-2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -41986,8 +42692,11 @@
       <c r="Q235">
         <v>4.13281E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R235">
+        <v>4.09541E-2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -42039,8 +42748,11 @@
       <c r="Q236">
         <v>2.0118200000000002</v>
       </c>
-    </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R236">
+        <v>2.04061</v>
+      </c>
+    </row>
+    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -42092,8 +42804,11 @@
       <c r="Q237">
         <v>11.4786</v>
       </c>
-    </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R237">
+        <v>11.472200000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -42145,8 +42860,11 @@
       <c r="Q238">
         <v>0.58557199999999998</v>
       </c>
-    </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R238">
+        <v>0.58426999999999996</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -42198,8 +42916,11 @@
       <c r="Q239">
         <v>1.1395</v>
       </c>
-    </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R239">
+        <v>1.1386099999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -42251,8 +42972,11 @@
       <c r="Q240">
         <v>0.98344399999999998</v>
       </c>
-    </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R240">
+        <v>0.98684300000000003</v>
+      </c>
+    </row>
+    <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -42304,8 +43028,11 @@
       <c r="Q241">
         <v>0.160798</v>
       </c>
-    </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R241">
+        <v>0.159526</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -42357,8 +43084,11 @@
       <c r="Q242">
         <v>0.112014</v>
       </c>
-    </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R242">
+        <v>0.113916</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -42410,8 +43140,11 @@
       <c r="Q243">
         <v>0.34176600000000001</v>
       </c>
-    </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R243">
+        <v>0.344032</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -42463,8 +43196,11 @@
       <c r="Q244">
         <v>1.7000599999999999</v>
       </c>
-    </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R244">
+        <v>1.6989300000000001</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -42516,8 +43252,11 @@
       <c r="Q245">
         <v>1.68249</v>
       </c>
-    </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R245">
+        <v>1.67533</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -42569,8 +43308,11 @@
       <c r="Q246">
         <v>0.100754</v>
       </c>
-    </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R246">
+        <v>0.100754</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -42622,8 +43364,11 @@
       <c r="Q247">
         <v>4.7796100000000001E-2</v>
       </c>
-    </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R247">
+        <v>4.8150100000000001E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -42675,8 +43420,11 @@
       <c r="Q248">
         <v>11.4617</v>
       </c>
-    </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R248">
+        <v>11.4633</v>
+      </c>
+    </row>
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -42728,8 +43476,11 @@
       <c r="Q249">
         <v>1.8368800000000001</v>
       </c>
-    </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R249">
+        <v>1.84276</v>
+      </c>
+    </row>
+    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -42781,8 +43532,11 @@
       <c r="Q250">
         <v>0.13805799999999999</v>
       </c>
-    </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R250">
+        <v>0.13778599999999999</v>
+      </c>
+    </row>
+    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -42834,8 +43588,11 @@
       <c r="Q251">
         <v>2.4426100000000002</v>
       </c>
-    </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R251">
+        <v>2.4402599999999999</v>
+      </c>
+    </row>
+    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -42887,8 +43644,11 @@
       <c r="Q252">
         <v>0.14488999999999999</v>
       </c>
-    </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R252">
+        <v>0.14357800000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -42940,8 +43700,11 @@
       <c r="Q253">
         <v>0.77322800000000003</v>
       </c>
-    </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R253">
+        <v>0.77815100000000004</v>
+      </c>
+    </row>
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -42993,8 +43756,11 @@
       <c r="Q254">
         <v>23.3262</v>
       </c>
-    </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R254">
+        <v>23.604399999999998</v>
+      </c>
+    </row>
+    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -43046,8 +43812,11 @@
       <c r="Q255">
         <v>1.02806</v>
       </c>
-    </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R255">
+        <v>1.03538</v>
+      </c>
+    </row>
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -43099,8 +43868,11 @@
       <c r="Q256">
         <v>0.51623600000000003</v>
       </c>
-    </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R256">
+        <v>0.52118200000000003</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -43152,8 +43924,11 @@
       <c r="Q257">
         <v>0.58590200000000003</v>
       </c>
-    </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R257">
+        <v>0.58775599999999995</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -43205,8 +43980,11 @@
       <c r="Q258">
         <v>2.81908</v>
       </c>
-    </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R258">
+        <v>2.8013300000000001</v>
+      </c>
+    </row>
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -43258,8 +44036,11 @@
       <c r="Q259">
         <v>23.8294</v>
       </c>
-    </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R259">
+        <v>23.782499999999999</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -43311,8 +44092,11 @@
       <c r="Q260">
         <v>1.40239</v>
       </c>
-    </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R260">
+        <v>1.4032100000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -43364,8 +44148,11 @@
       <c r="Q261">
         <v>0.58762000000000003</v>
       </c>
-    </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R261">
+        <v>0.59955800000000004</v>
+      </c>
+    </row>
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -43417,8 +44204,11 @@
       <c r="Q262">
         <v>0.48191600000000001</v>
       </c>
-    </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R262">
+        <v>0.48670600000000003</v>
+      </c>
+    </row>
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -43470,8 +44260,11 @@
       <c r="Q263">
         <v>9.0735899999999994E-2</v>
       </c>
-    </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R263">
+        <v>9.2851900000000001E-2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -43523,8 +44316,11 @@
       <c r="Q264">
         <v>1.6984699999999999</v>
       </c>
-    </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R264">
+        <v>1.7012499999999999</v>
+      </c>
+    </row>
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -43576,8 +44372,11 @@
       <c r="Q265">
         <v>0.98872199999999999</v>
       </c>
-    </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R265">
+        <v>0.99105299999999996</v>
+      </c>
+    </row>
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -43629,8 +44428,11 @@
       <c r="Q266">
         <v>0.80042199999999997</v>
       </c>
-    </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R266">
+        <v>0.79873499999999997</v>
+      </c>
+    </row>
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -43682,8 +44484,11 @@
       <c r="Q267">
         <v>0.21682000000000001</v>
       </c>
-    </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R267">
+        <v>0.21754100000000001</v>
+      </c>
+    </row>
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -43735,8 +44540,11 @@
       <c r="Q268">
         <v>0.97240000000000004</v>
       </c>
-    </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R268">
+        <v>0.973302</v>
+      </c>
+    </row>
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -43788,8 +44596,11 @@
       <c r="Q269">
         <v>2.2619099999999999</v>
       </c>
-    </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R269">
+        <v>2.2640899999999999</v>
+      </c>
+    </row>
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -43841,8 +44652,11 @@
       <c r="Q270">
         <v>11.4907</v>
       </c>
-    </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R270">
+        <v>11.489599999999999</v>
+      </c>
+    </row>
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -43894,8 +44708,11 @@
       <c r="Q271">
         <v>1.2920199999999999</v>
       </c>
-    </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R271">
+        <v>1.3035600000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -43947,8 +44764,11 @@
       <c r="Q272">
         <v>0.79962900000000003</v>
       </c>
-    </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R272">
+        <v>0.80619300000000005</v>
+      </c>
+    </row>
+    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -44000,8 +44820,11 @@
       <c r="Q273">
         <v>0.72397800000000001</v>
       </c>
-    </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R273">
+        <v>0.72691499999999998</v>
+      </c>
+    </row>
+    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -44053,8 +44876,11 @@
       <c r="Q274">
         <v>0.51543399999999995</v>
       </c>
-    </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R274">
+        <v>0.51663199999999998</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -44106,8 +44932,11 @@
       <c r="Q275">
         <v>4.9584000000000003E-2</v>
       </c>
-    </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R275">
+        <v>5.0051999999999999E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -44159,8 +44988,11 @@
       <c r="Q276">
         <v>0.59478600000000004</v>
       </c>
-    </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R276">
+        <v>0.58909599999999995</v>
+      </c>
+    </row>
+    <row r="277" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -44212,8 +45044,11 @@
       <c r="Q277">
         <v>0.87702800000000003</v>
       </c>
-    </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R277">
+        <v>0.872587</v>
+      </c>
+    </row>
+    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -44265,8 +45100,11 @@
       <c r="Q278">
         <v>0.81823599999999996</v>
       </c>
-    </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R278">
+        <v>0.82293099999999997</v>
+      </c>
+    </row>
+    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -44318,8 +45156,11 @@
       <c r="Q279">
         <v>1.30768</v>
       </c>
-    </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R279">
+        <v>1.3119099999999999</v>
+      </c>
+    </row>
+    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -44371,8 +45212,11 @@
       <c r="Q280">
         <v>0.58217799999999997</v>
       </c>
-    </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R280">
+        <v>0.57799599999999995</v>
+      </c>
+    </row>
+    <row r="281" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -44424,8 +45268,11 @@
       <c r="Q281">
         <v>11.4756</v>
       </c>
-    </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R281">
+        <v>11.458399999999999</v>
+      </c>
+    </row>
+    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -44477,8 +45324,11 @@
       <c r="Q282">
         <v>0.53304399999999996</v>
       </c>
-    </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R282">
+        <v>0.53263400000000005</v>
+      </c>
+    </row>
+    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -44530,8 +45380,11 @@
       <c r="Q283">
         <v>0.120492</v>
       </c>
-    </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R283">
+        <v>0.120586</v>
+      </c>
+    </row>
+    <row r="284" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -44583,8 +45436,11 @@
       <c r="Q284">
         <v>0.47855399999999998</v>
       </c>
-    </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R284">
+        <v>0.47897000000000001</v>
+      </c>
+    </row>
+    <row r="285" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -44636,8 +45492,11 @@
       <c r="Q285">
         <v>0.43792599999999998</v>
       </c>
-    </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R285">
+        <v>0.443276</v>
+      </c>
+    </row>
+    <row r="286" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -44689,8 +45548,11 @@
       <c r="Q286">
         <v>0.236147</v>
       </c>
-    </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R286">
+        <v>0.238149</v>
+      </c>
+    </row>
+    <row r="287" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -44742,8 +45604,11 @@
       <c r="Q287">
         <v>0.40125</v>
       </c>
-    </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R287">
+        <v>0.40516400000000002</v>
+      </c>
+    </row>
+    <row r="288" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -44795,8 +45660,11 @@
       <c r="Q288">
         <v>6.8596199999999996E-2</v>
       </c>
-    </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R288">
+        <v>6.9326200000000004E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -44848,8 +45716,11 @@
       <c r="Q289">
         <v>0.63990800000000003</v>
       </c>
-    </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R289">
+        <v>0.64416300000000004</v>
+      </c>
+    </row>
+    <row r="290" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -44901,8 +45772,11 @@
       <c r="Q290">
         <v>0.92511600000000005</v>
       </c>
-    </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R290">
+        <v>0.93669000000000002</v>
+      </c>
+    </row>
+    <row r="291" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -44954,8 +45828,11 @@
       <c r="Q291">
         <v>0.52854800000000002</v>
       </c>
-    </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R291">
+        <v>0.52806200000000003</v>
+      </c>
+    </row>
+    <row r="292" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>291</v>
       </c>
@@ -45003,6 +45880,9 @@
       </c>
       <c r="Q292" t="s">
         <v>306</v>
+      </c>
+      <c r="R292" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>